<commit_message>
Project GACC_Final_Prod is saved. Fixed null issue Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/GACC_Final_Prod/GACC_Rating_Model.xlsx
+++ b/DESIGN/rules/GACC_Final_Prod/GACC_Rating_Model.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n0206863/Downloads/GACC-5.21.12_25032019/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FD1D24-4454-4A44-93CB-A93B0D7ACFC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="14620" windowWidth="23260" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="14625" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -47,12 +41,12 @@
     <definedName name="State">[1]Inputs!$C$21</definedName>
     <definedName name="Termination_Age">[1]Inputs!$C$42</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="400">
   <si>
     <r>
       <rPr>
@@ -2357,21 +2351,30 @@
   </si>
   <si>
     <t>com.lmig.grm.ag.openlgen</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>org.openl.rules.binding.MulDivNullToOneOperators.*</t>
+  </si>
+  <si>
+    <t>Environment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="8">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0;\(#,##0.0\)"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00;\(#,##0.00\)"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0"/>
-    <numFmt numFmtId="168" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
-    <numFmt numFmtId="169" formatCode="0%;\(0%\)"/>
-    <numFmt numFmtId="170" formatCode="0.0%;\(0.0%\)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0;\(#,##0.0\)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;\(#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="168" formatCode="0%;\(0%\)"/>
+    <numFmt numFmtId="169" formatCode="0.0%;\(0.0%\)"/>
   </numFmts>
   <fonts count="76">
     <font>
@@ -3487,7 +3490,7 @@
     <xf numFmtId="1" fontId="25" fillId="0" borderId="0" applyFont="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" applyFont="0"/>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3500,7 +3503,7 @@
     <xf numFmtId="0" fontId="27" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" applyFont="0"/>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" applyFont="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3558,7 +3561,7 @@
     <xf numFmtId="3" fontId="33" fillId="0" borderId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="0">
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="43" fontId="34" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3777,13 +3780,13 @@
     <xf numFmtId="43" fontId="34" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="36" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="36" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="41" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4356,17 +4359,17 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="36" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="26" fillId="0" borderId="0" applyFont="0"/>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="0" applyFont="0">
+    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" applyFont="0"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" applyFont="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="0" applyFont="0">
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" applyFont="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="0" applyFont="0">
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" applyFont="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="0" applyFont="0">
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" applyFont="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0">
@@ -4518,6 +4521,15 @@
     <xf numFmtId="0" fontId="73" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="25" xfId="914" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="75" fillId="33" borderId="25" xfId="914" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="26" xfId="914" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4533,932 +4545,923 @@
     <xf numFmtId="0" fontId="74" fillId="56" borderId="25" xfId="914" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="25" xfId="914" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="75" fillId="33" borderId="25" xfId="914" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="26" xfId="914" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="915">
-    <cellStyle name="0DECIMAL" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="0DECIMAL 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="0DECIMAL 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="0DECIMAL 2 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="1DECIMAL" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="0DECIMAL" xfId="3"/>
+    <cellStyle name="0DECIMAL 2" xfId="4"/>
+    <cellStyle name="0DECIMAL 2 2" xfId="5"/>
+    <cellStyle name="0DECIMAL 2 3" xfId="6"/>
+    <cellStyle name="1DECIMAL" xfId="7"/>
     <cellStyle name="20% - Accent1" xfId="886" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="20% - Accent1 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="8"/>
+    <cellStyle name="20% - Accent1 2 2" xfId="9"/>
     <cellStyle name="20% - Accent2" xfId="890" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - Accent2 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="10"/>
+    <cellStyle name="20% - Accent2 2 2" xfId="11"/>
     <cellStyle name="20% - Accent3" xfId="894" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="20% - Accent3 2 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="12"/>
+    <cellStyle name="20% - Accent3 2 2" xfId="13"/>
     <cellStyle name="20% - Accent4" xfId="898" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="20% - Accent4 2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="14"/>
+    <cellStyle name="20% - Accent4 2 2" xfId="15"/>
     <cellStyle name="20% - Accent5" xfId="902" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="20% - Accent5 2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="16"/>
+    <cellStyle name="20% - Accent5 2 2" xfId="17"/>
     <cellStyle name="20% - Accent6" xfId="906" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="20% - Accent6 2 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="2DECIMAL" xfId="20" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="18"/>
+    <cellStyle name="20% - Accent6 2 2" xfId="19"/>
+    <cellStyle name="2DECIMAL" xfId="20"/>
     <cellStyle name="40% - Accent1" xfId="887" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="40% - Accent1 2 2" xfId="22" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="21"/>
+    <cellStyle name="40% - Accent1 2 2" xfId="22"/>
     <cellStyle name="40% - Accent2" xfId="891" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="40% - Accent2 2 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="23"/>
+    <cellStyle name="40% - Accent2 2 2" xfId="24"/>
     <cellStyle name="40% - Accent3" xfId="895" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="40% - Accent3 2 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="25"/>
+    <cellStyle name="40% - Accent3 2 2" xfId="26"/>
     <cellStyle name="40% - Accent4" xfId="899" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="40% - Accent4 2 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="27"/>
+    <cellStyle name="40% - Accent4 2 2" xfId="28"/>
     <cellStyle name="40% - Accent5" xfId="903" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="40% - Accent5 2 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="29"/>
+    <cellStyle name="40% - Accent5 2 2" xfId="30"/>
     <cellStyle name="40% - Accent6" xfId="907" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="40% - Accent6 2 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="31"/>
+    <cellStyle name="40% - Accent6 2 2" xfId="32"/>
     <cellStyle name="60% - Accent1" xfId="888" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="60% - Accent1 2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="33"/>
+    <cellStyle name="60% - Accent1 2 2" xfId="34"/>
     <cellStyle name="60% - Accent2" xfId="892" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2 2" xfId="35" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="60% - Accent2 2 2" xfId="36" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="35"/>
+    <cellStyle name="60% - Accent2 2 2" xfId="36"/>
     <cellStyle name="60% - Accent3" xfId="896" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="60% - Accent3 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="37"/>
+    <cellStyle name="60% - Accent3 2 2" xfId="38"/>
     <cellStyle name="60% - Accent4" xfId="900" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="60% - Accent4 2 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="39"/>
+    <cellStyle name="60% - Accent4 2 2" xfId="40"/>
     <cellStyle name="60% - Accent5" xfId="904" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="60% - Accent5 2 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="41"/>
+    <cellStyle name="60% - Accent5 2 2" xfId="42"/>
     <cellStyle name="60% - Accent6" xfId="908" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="60% - Accent6 2 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="43"/>
+    <cellStyle name="60% - Accent6 2 2" xfId="44"/>
     <cellStyle name="Accent1" xfId="885" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent1 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Accent1 2 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Accent1 2" xfId="45"/>
+    <cellStyle name="Accent1 2 2" xfId="46"/>
     <cellStyle name="Accent2" xfId="889" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Accent2 2 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Accent2 2" xfId="47"/>
+    <cellStyle name="Accent2 2 2" xfId="48"/>
     <cellStyle name="Accent3" xfId="893" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent3 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Accent3 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Accent3 2" xfId="49"/>
+    <cellStyle name="Accent3 2 2" xfId="50"/>
     <cellStyle name="Accent4" xfId="897" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent4 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Accent4 2 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Accent4 2" xfId="51"/>
+    <cellStyle name="Accent4 2 2" xfId="52"/>
     <cellStyle name="Accent5" xfId="901" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent5 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Accent5 2 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Accent5 2" xfId="53"/>
+    <cellStyle name="Accent5 2 2" xfId="54"/>
     <cellStyle name="Accent6" xfId="905" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Accent6 2" xfId="55" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Accent6 2 2" xfId="56" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Accent6 2" xfId="55"/>
+    <cellStyle name="Accent6 2 2" xfId="56"/>
     <cellStyle name="Bad" xfId="874" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Bad 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Bad 2 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Bad 2" xfId="57"/>
+    <cellStyle name="Bad 2 2" xfId="58"/>
     <cellStyle name="Calculation" xfId="878" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Calculation 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Calculation 2 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Calculation 2 2 2" xfId="909" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Calculation 2" xfId="59"/>
+    <cellStyle name="Calculation 2 2" xfId="60"/>
+    <cellStyle name="Calculation 2 2 2" xfId="909"/>
     <cellStyle name="Check Cell" xfId="880" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Check Cell 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Check Cell 2 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="column heading border A&amp;B" xfId="63" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="column heading border above" xfId="64" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="column heading border below" xfId="65" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="column heading no border &amp; short title" xfId="66" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="comma 0 decimal" xfId="67" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="comma 1 decimal" xfId="68" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Comma 10" xfId="69" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Comma 2" xfId="70" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Comma 2 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Comma 2 2 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Comma 2 3" xfId="73" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Comma 2 4" xfId="74" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Comma 2 5" xfId="75" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Comma 2 5 2" xfId="76" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Comma 2 6" xfId="77" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Comma 2 7" xfId="78" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="comma 2 decimal" xfId="79" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Comma 3" xfId="80" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Comma 3 10" xfId="81" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Comma 3 11" xfId="82" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Comma 3 2" xfId="83" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Comma 3 3" xfId="84" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Comma 3 3 2" xfId="85" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Comma 3 3 2 2" xfId="86" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Comma 3 3 2 2 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Comma 3 3 2 2 2 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Comma 3 3 2 2 2 2 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Comma 3 3 2 2 2 3" xfId="90" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Comma 3 3 2 2 2 4" xfId="91" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Comma 3 3 2 2 2 5" xfId="92" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Comma 3 3 2 2 3" xfId="93" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Comma 3 3 2 2 3 2" xfId="94" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Comma 3 3 2 2 4" xfId="95" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Comma 3 3 2 2 5" xfId="96" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Comma 3 3 2 2 6" xfId="97" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Comma 3 3 2 3" xfId="98" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Comma 3 3 2 3 2" xfId="99" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Comma 3 3 2 3 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Comma 3 3 2 3 3" xfId="101" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Comma 3 3 2 3 4" xfId="102" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Comma 3 3 2 3 5" xfId="103" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Comma 3 3 2 4" xfId="104" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Comma 3 3 2 4 2" xfId="105" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Comma 3 3 2 5" xfId="106" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Comma 3 3 2 6" xfId="107" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Comma 3 3 2 7" xfId="108" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Comma 3 3 3" xfId="109" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Comma 3 3 3 2" xfId="110" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Comma 3 3 3 2 2" xfId="111" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Comma 3 3 3 2 2 2" xfId="112" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Comma 3 3 3 2 3" xfId="113" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Comma 3 3 3 2 4" xfId="114" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Comma 3 3 3 2 5" xfId="115" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Comma 3 3 3 3" xfId="116" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Comma 3 3 3 3 2" xfId="117" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Comma 3 3 3 4" xfId="118" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Comma 3 3 3 5" xfId="119" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Comma 3 3 3 6" xfId="120" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Comma 3 3 4" xfId="121" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Comma 3 3 4 2" xfId="122" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Comma 3 3 4 2 2" xfId="123" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Comma 3 3 4 3" xfId="124" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Comma 3 3 4 4" xfId="125" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Comma 3 3 4 5" xfId="126" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Comma 3 3 5" xfId="127" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Comma 3 3 5 2" xfId="128" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="Comma 3 3 6" xfId="129" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="Comma 3 3 7" xfId="130" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="Comma 3 3 8" xfId="131" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="Comma 3 4" xfId="132" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="Comma 3 4 2" xfId="133" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="Comma 3 4 2 2" xfId="134" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="Comma 3 4 2 2 2" xfId="135" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="Comma 3 4 2 2 2 2" xfId="136" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="Comma 3 4 2 2 3" xfId="137" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="Comma 3 4 2 2 4" xfId="138" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="Comma 3 4 2 2 5" xfId="139" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="Comma 3 4 2 3" xfId="140" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
-    <cellStyle name="Comma 3 4 2 3 2" xfId="141" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
-    <cellStyle name="Comma 3 4 2 4" xfId="142" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
-    <cellStyle name="Comma 3 4 2 5" xfId="143" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
-    <cellStyle name="Comma 3 4 2 6" xfId="144" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
-    <cellStyle name="Comma 3 4 3" xfId="145" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
-    <cellStyle name="Comma 3 4 3 2" xfId="146" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
-    <cellStyle name="Comma 3 4 3 2 2" xfId="147" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
-    <cellStyle name="Comma 3 4 3 3" xfId="148" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
-    <cellStyle name="Comma 3 4 3 4" xfId="149" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
-    <cellStyle name="Comma 3 4 3 5" xfId="150" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
-    <cellStyle name="Comma 3 4 4" xfId="151" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
-    <cellStyle name="Comma 3 4 4 2" xfId="152" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
-    <cellStyle name="Comma 3 4 5" xfId="153" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
-    <cellStyle name="Comma 3 4 6" xfId="154" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
-    <cellStyle name="Comma 3 4 7" xfId="155" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
-    <cellStyle name="Comma 3 5" xfId="156" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
-    <cellStyle name="Comma 3 5 2" xfId="157" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
-    <cellStyle name="Comma 3 5 2 2" xfId="158" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
-    <cellStyle name="Comma 3 5 2 2 2" xfId="159" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="Comma 3 5 2 3" xfId="160" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
-    <cellStyle name="Comma 3 5 2 4" xfId="161" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
-    <cellStyle name="Comma 3 5 2 5" xfId="162" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
-    <cellStyle name="Comma 3 5 3" xfId="163" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
-    <cellStyle name="Comma 3 5 3 2" xfId="164" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="Comma 3 5 4" xfId="165" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
-    <cellStyle name="Comma 3 5 5" xfId="166" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
-    <cellStyle name="Comma 3 5 6" xfId="167" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
-    <cellStyle name="Comma 3 6" xfId="168" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
-    <cellStyle name="Comma 3 6 2" xfId="169" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
-    <cellStyle name="Comma 3 6 2 2" xfId="170" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
-    <cellStyle name="Comma 3 6 3" xfId="171" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
-    <cellStyle name="Comma 3 6 4" xfId="172" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
-    <cellStyle name="Comma 3 6 5" xfId="173" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
-    <cellStyle name="Comma 3 7" xfId="174" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
-    <cellStyle name="Comma 3 8" xfId="175" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
-    <cellStyle name="Comma 3 8 2" xfId="176" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
-    <cellStyle name="Comma 3 9" xfId="177" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
-    <cellStyle name="Comma 4" xfId="178" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="Comma 4 10" xfId="179" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
-    <cellStyle name="Comma 4 11" xfId="180" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
-    <cellStyle name="Comma 4 12" xfId="181" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
-    <cellStyle name="Comma 4 2" xfId="182" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
-    <cellStyle name="Comma 4 3" xfId="183" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
-    <cellStyle name="Comma 4 4" xfId="184" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
-    <cellStyle name="Comma 4 5" xfId="185" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
-    <cellStyle name="Comma 4 5 2" xfId="186" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
-    <cellStyle name="Comma 4 5 2 2" xfId="187" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
-    <cellStyle name="Comma 4 5 2 2 2" xfId="188" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
-    <cellStyle name="Comma 4 5 2 2 2 2" xfId="189" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
-    <cellStyle name="Comma 4 5 2 2 2 2 2" xfId="190" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
-    <cellStyle name="Comma 4 5 2 2 2 3" xfId="191" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
-    <cellStyle name="Comma 4 5 2 2 2 4" xfId="192" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
-    <cellStyle name="Comma 4 5 2 2 2 5" xfId="193" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
-    <cellStyle name="Comma 4 5 2 2 3" xfId="194" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
-    <cellStyle name="Comma 4 5 2 2 3 2" xfId="195" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
-    <cellStyle name="Comma 4 5 2 2 4" xfId="196" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
-    <cellStyle name="Comma 4 5 2 2 5" xfId="197" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
-    <cellStyle name="Comma 4 5 2 2 6" xfId="198" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
-    <cellStyle name="Comma 4 5 2 3" xfId="199" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
-    <cellStyle name="Comma 4 5 2 3 2" xfId="200" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
-    <cellStyle name="Comma 4 5 2 3 2 2" xfId="201" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
-    <cellStyle name="Comma 4 5 2 3 3" xfId="202" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
-    <cellStyle name="Comma 4 5 2 3 4" xfId="203" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
-    <cellStyle name="Comma 4 5 2 3 5" xfId="204" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
-    <cellStyle name="Comma 4 5 2 4" xfId="205" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
-    <cellStyle name="Comma 4 5 2 4 2" xfId="206" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
-    <cellStyle name="Comma 4 5 2 5" xfId="207" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
-    <cellStyle name="Comma 4 5 2 6" xfId="208" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
-    <cellStyle name="Comma 4 5 2 7" xfId="209" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
-    <cellStyle name="Comma 4 5 3" xfId="210" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
-    <cellStyle name="Comma 4 5 3 2" xfId="211" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
-    <cellStyle name="Comma 4 5 3 2 2" xfId="212" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
-    <cellStyle name="Comma 4 5 3 2 2 2" xfId="213" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
-    <cellStyle name="Comma 4 5 3 2 3" xfId="214" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
-    <cellStyle name="Comma 4 5 3 2 4" xfId="215" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
-    <cellStyle name="Comma 4 5 3 2 5" xfId="216" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
-    <cellStyle name="Comma 4 5 3 3" xfId="217" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
-    <cellStyle name="Comma 4 5 3 3 2" xfId="218" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
-    <cellStyle name="Comma 4 5 3 4" xfId="219" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
-    <cellStyle name="Comma 4 5 3 5" xfId="220" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
-    <cellStyle name="Comma 4 5 3 6" xfId="221" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
-    <cellStyle name="Comma 4 5 4" xfId="222" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
-    <cellStyle name="Comma 4 5 4 2" xfId="223" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
-    <cellStyle name="Comma 4 5 4 2 2" xfId="224" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
-    <cellStyle name="Comma 4 5 4 3" xfId="225" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
-    <cellStyle name="Comma 4 5 4 4" xfId="226" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
-    <cellStyle name="Comma 4 5 4 5" xfId="227" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
-    <cellStyle name="Comma 4 5 5" xfId="228" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
-    <cellStyle name="Comma 4 5 5 2" xfId="229" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
-    <cellStyle name="Comma 4 5 6" xfId="230" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
-    <cellStyle name="Comma 4 5 7" xfId="231" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
-    <cellStyle name="Comma 4 5 8" xfId="232" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
-    <cellStyle name="Comma 4 6" xfId="233" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
-    <cellStyle name="Comma 4 6 2" xfId="234" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
-    <cellStyle name="Comma 4 6 2 2" xfId="235" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
-    <cellStyle name="Comma 4 6 2 2 2" xfId="236" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
-    <cellStyle name="Comma 4 6 2 2 2 2" xfId="237" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
-    <cellStyle name="Comma 4 6 2 2 3" xfId="238" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
-    <cellStyle name="Comma 4 6 2 2 4" xfId="239" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
-    <cellStyle name="Comma 4 6 2 2 5" xfId="240" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
-    <cellStyle name="Comma 4 6 2 3" xfId="241" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
-    <cellStyle name="Comma 4 6 2 3 2" xfId="242" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
-    <cellStyle name="Comma 4 6 2 4" xfId="243" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
-    <cellStyle name="Comma 4 6 2 5" xfId="244" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
-    <cellStyle name="Comma 4 6 2 6" xfId="245" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
-    <cellStyle name="Comma 4 6 3" xfId="246" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
-    <cellStyle name="Comma 4 6 3 2" xfId="247" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
-    <cellStyle name="Comma 4 6 3 2 2" xfId="248" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
-    <cellStyle name="Comma 4 6 3 3" xfId="249" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
-    <cellStyle name="Comma 4 6 3 4" xfId="250" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
-    <cellStyle name="Comma 4 6 3 5" xfId="251" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
-    <cellStyle name="Comma 4 6 4" xfId="252" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
-    <cellStyle name="Comma 4 6 4 2" xfId="253" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
-    <cellStyle name="Comma 4 6 5" xfId="254" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
-    <cellStyle name="Comma 4 6 6" xfId="255" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
-    <cellStyle name="Comma 4 6 7" xfId="256" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
-    <cellStyle name="Comma 4 7" xfId="257" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
-    <cellStyle name="Comma 4 7 2" xfId="258" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
-    <cellStyle name="Comma 4 7 2 2" xfId="259" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
-    <cellStyle name="Comma 4 7 2 2 2" xfId="260" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
-    <cellStyle name="Comma 4 7 2 3" xfId="261" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
-    <cellStyle name="Comma 4 7 2 4" xfId="262" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
-    <cellStyle name="Comma 4 7 2 5" xfId="263" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
-    <cellStyle name="Comma 4 7 3" xfId="264" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
-    <cellStyle name="Comma 4 7 3 2" xfId="265" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
-    <cellStyle name="Comma 4 7 4" xfId="266" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
-    <cellStyle name="Comma 4 7 5" xfId="267" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
-    <cellStyle name="Comma 4 7 6" xfId="268" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
-    <cellStyle name="Comma 4 8" xfId="269" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
-    <cellStyle name="Comma 4 8 2" xfId="270" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
-    <cellStyle name="Comma 4 8 2 2" xfId="271" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
-    <cellStyle name="Comma 4 8 3" xfId="272" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
-    <cellStyle name="Comma 4 8 4" xfId="273" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
-    <cellStyle name="Comma 4 8 5" xfId="274" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
-    <cellStyle name="Comma 4 9" xfId="275" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
-    <cellStyle name="Comma 4 9 2" xfId="276" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
-    <cellStyle name="Comma 5" xfId="277" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
-    <cellStyle name="Comma 5 2" xfId="278" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
-    <cellStyle name="Comma 6" xfId="279" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
-    <cellStyle name="Comma 7" xfId="280" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
-    <cellStyle name="Comma 8" xfId="281" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
-    <cellStyle name="Comma 9" xfId="282" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
-    <cellStyle name="Currency 2" xfId="283" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
-    <cellStyle name="Currency 2 2" xfId="284" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
-    <cellStyle name="Currency 2 3" xfId="285" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
-    <cellStyle name="Currency 3" xfId="286" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
-    <cellStyle name="Datatype" xfId="2" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
-    <cellStyle name="Euro" xfId="287" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
-    <cellStyle name="Euro 2" xfId="288" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
-    <cellStyle name="Euro 2 2" xfId="289" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Check Cell 2" xfId="61"/>
+    <cellStyle name="Check Cell 2 2" xfId="62"/>
+    <cellStyle name="column heading border A&amp;B" xfId="63"/>
+    <cellStyle name="column heading border above" xfId="64"/>
+    <cellStyle name="column heading border below" xfId="65"/>
+    <cellStyle name="column heading no border &amp; short title" xfId="66"/>
+    <cellStyle name="comma 0 decimal" xfId="67"/>
+    <cellStyle name="comma 1 decimal" xfId="68"/>
+    <cellStyle name="Comma 10" xfId="69"/>
+    <cellStyle name="Comma 2" xfId="70"/>
+    <cellStyle name="Comma 2 2" xfId="71"/>
+    <cellStyle name="Comma 2 2 2" xfId="72"/>
+    <cellStyle name="Comma 2 3" xfId="73"/>
+    <cellStyle name="Comma 2 4" xfId="74"/>
+    <cellStyle name="Comma 2 5" xfId="75"/>
+    <cellStyle name="Comma 2 5 2" xfId="76"/>
+    <cellStyle name="Comma 2 6" xfId="77"/>
+    <cellStyle name="Comma 2 7" xfId="78"/>
+    <cellStyle name="comma 2 decimal" xfId="79"/>
+    <cellStyle name="Comma 3" xfId="80"/>
+    <cellStyle name="Comma 3 10" xfId="81"/>
+    <cellStyle name="Comma 3 11" xfId="82"/>
+    <cellStyle name="Comma 3 2" xfId="83"/>
+    <cellStyle name="Comma 3 3" xfId="84"/>
+    <cellStyle name="Comma 3 3 2" xfId="85"/>
+    <cellStyle name="Comma 3 3 2 2" xfId="86"/>
+    <cellStyle name="Comma 3 3 2 2 2" xfId="87"/>
+    <cellStyle name="Comma 3 3 2 2 2 2" xfId="88"/>
+    <cellStyle name="Comma 3 3 2 2 2 2 2" xfId="89"/>
+    <cellStyle name="Comma 3 3 2 2 2 3" xfId="90"/>
+    <cellStyle name="Comma 3 3 2 2 2 4" xfId="91"/>
+    <cellStyle name="Comma 3 3 2 2 2 5" xfId="92"/>
+    <cellStyle name="Comma 3 3 2 2 3" xfId="93"/>
+    <cellStyle name="Comma 3 3 2 2 3 2" xfId="94"/>
+    <cellStyle name="Comma 3 3 2 2 4" xfId="95"/>
+    <cellStyle name="Comma 3 3 2 2 5" xfId="96"/>
+    <cellStyle name="Comma 3 3 2 2 6" xfId="97"/>
+    <cellStyle name="Comma 3 3 2 3" xfId="98"/>
+    <cellStyle name="Comma 3 3 2 3 2" xfId="99"/>
+    <cellStyle name="Comma 3 3 2 3 2 2" xfId="100"/>
+    <cellStyle name="Comma 3 3 2 3 3" xfId="101"/>
+    <cellStyle name="Comma 3 3 2 3 4" xfId="102"/>
+    <cellStyle name="Comma 3 3 2 3 5" xfId="103"/>
+    <cellStyle name="Comma 3 3 2 4" xfId="104"/>
+    <cellStyle name="Comma 3 3 2 4 2" xfId="105"/>
+    <cellStyle name="Comma 3 3 2 5" xfId="106"/>
+    <cellStyle name="Comma 3 3 2 6" xfId="107"/>
+    <cellStyle name="Comma 3 3 2 7" xfId="108"/>
+    <cellStyle name="Comma 3 3 3" xfId="109"/>
+    <cellStyle name="Comma 3 3 3 2" xfId="110"/>
+    <cellStyle name="Comma 3 3 3 2 2" xfId="111"/>
+    <cellStyle name="Comma 3 3 3 2 2 2" xfId="112"/>
+    <cellStyle name="Comma 3 3 3 2 3" xfId="113"/>
+    <cellStyle name="Comma 3 3 3 2 4" xfId="114"/>
+    <cellStyle name="Comma 3 3 3 2 5" xfId="115"/>
+    <cellStyle name="Comma 3 3 3 3" xfId="116"/>
+    <cellStyle name="Comma 3 3 3 3 2" xfId="117"/>
+    <cellStyle name="Comma 3 3 3 4" xfId="118"/>
+    <cellStyle name="Comma 3 3 3 5" xfId="119"/>
+    <cellStyle name="Comma 3 3 3 6" xfId="120"/>
+    <cellStyle name="Comma 3 3 4" xfId="121"/>
+    <cellStyle name="Comma 3 3 4 2" xfId="122"/>
+    <cellStyle name="Comma 3 3 4 2 2" xfId="123"/>
+    <cellStyle name="Comma 3 3 4 3" xfId="124"/>
+    <cellStyle name="Comma 3 3 4 4" xfId="125"/>
+    <cellStyle name="Comma 3 3 4 5" xfId="126"/>
+    <cellStyle name="Comma 3 3 5" xfId="127"/>
+    <cellStyle name="Comma 3 3 5 2" xfId="128"/>
+    <cellStyle name="Comma 3 3 6" xfId="129"/>
+    <cellStyle name="Comma 3 3 7" xfId="130"/>
+    <cellStyle name="Comma 3 3 8" xfId="131"/>
+    <cellStyle name="Comma 3 4" xfId="132"/>
+    <cellStyle name="Comma 3 4 2" xfId="133"/>
+    <cellStyle name="Comma 3 4 2 2" xfId="134"/>
+    <cellStyle name="Comma 3 4 2 2 2" xfId="135"/>
+    <cellStyle name="Comma 3 4 2 2 2 2" xfId="136"/>
+    <cellStyle name="Comma 3 4 2 2 3" xfId="137"/>
+    <cellStyle name="Comma 3 4 2 2 4" xfId="138"/>
+    <cellStyle name="Comma 3 4 2 2 5" xfId="139"/>
+    <cellStyle name="Comma 3 4 2 3" xfId="140"/>
+    <cellStyle name="Comma 3 4 2 3 2" xfId="141"/>
+    <cellStyle name="Comma 3 4 2 4" xfId="142"/>
+    <cellStyle name="Comma 3 4 2 5" xfId="143"/>
+    <cellStyle name="Comma 3 4 2 6" xfId="144"/>
+    <cellStyle name="Comma 3 4 3" xfId="145"/>
+    <cellStyle name="Comma 3 4 3 2" xfId="146"/>
+    <cellStyle name="Comma 3 4 3 2 2" xfId="147"/>
+    <cellStyle name="Comma 3 4 3 3" xfId="148"/>
+    <cellStyle name="Comma 3 4 3 4" xfId="149"/>
+    <cellStyle name="Comma 3 4 3 5" xfId="150"/>
+    <cellStyle name="Comma 3 4 4" xfId="151"/>
+    <cellStyle name="Comma 3 4 4 2" xfId="152"/>
+    <cellStyle name="Comma 3 4 5" xfId="153"/>
+    <cellStyle name="Comma 3 4 6" xfId="154"/>
+    <cellStyle name="Comma 3 4 7" xfId="155"/>
+    <cellStyle name="Comma 3 5" xfId="156"/>
+    <cellStyle name="Comma 3 5 2" xfId="157"/>
+    <cellStyle name="Comma 3 5 2 2" xfId="158"/>
+    <cellStyle name="Comma 3 5 2 2 2" xfId="159"/>
+    <cellStyle name="Comma 3 5 2 3" xfId="160"/>
+    <cellStyle name="Comma 3 5 2 4" xfId="161"/>
+    <cellStyle name="Comma 3 5 2 5" xfId="162"/>
+    <cellStyle name="Comma 3 5 3" xfId="163"/>
+    <cellStyle name="Comma 3 5 3 2" xfId="164"/>
+    <cellStyle name="Comma 3 5 4" xfId="165"/>
+    <cellStyle name="Comma 3 5 5" xfId="166"/>
+    <cellStyle name="Comma 3 5 6" xfId="167"/>
+    <cellStyle name="Comma 3 6" xfId="168"/>
+    <cellStyle name="Comma 3 6 2" xfId="169"/>
+    <cellStyle name="Comma 3 6 2 2" xfId="170"/>
+    <cellStyle name="Comma 3 6 3" xfId="171"/>
+    <cellStyle name="Comma 3 6 4" xfId="172"/>
+    <cellStyle name="Comma 3 6 5" xfId="173"/>
+    <cellStyle name="Comma 3 7" xfId="174"/>
+    <cellStyle name="Comma 3 8" xfId="175"/>
+    <cellStyle name="Comma 3 8 2" xfId="176"/>
+    <cellStyle name="Comma 3 9" xfId="177"/>
+    <cellStyle name="Comma 4" xfId="178"/>
+    <cellStyle name="Comma 4 10" xfId="179"/>
+    <cellStyle name="Comma 4 11" xfId="180"/>
+    <cellStyle name="Comma 4 12" xfId="181"/>
+    <cellStyle name="Comma 4 2" xfId="182"/>
+    <cellStyle name="Comma 4 3" xfId="183"/>
+    <cellStyle name="Comma 4 4" xfId="184"/>
+    <cellStyle name="Comma 4 5" xfId="185"/>
+    <cellStyle name="Comma 4 5 2" xfId="186"/>
+    <cellStyle name="Comma 4 5 2 2" xfId="187"/>
+    <cellStyle name="Comma 4 5 2 2 2" xfId="188"/>
+    <cellStyle name="Comma 4 5 2 2 2 2" xfId="189"/>
+    <cellStyle name="Comma 4 5 2 2 2 2 2" xfId="190"/>
+    <cellStyle name="Comma 4 5 2 2 2 3" xfId="191"/>
+    <cellStyle name="Comma 4 5 2 2 2 4" xfId="192"/>
+    <cellStyle name="Comma 4 5 2 2 2 5" xfId="193"/>
+    <cellStyle name="Comma 4 5 2 2 3" xfId="194"/>
+    <cellStyle name="Comma 4 5 2 2 3 2" xfId="195"/>
+    <cellStyle name="Comma 4 5 2 2 4" xfId="196"/>
+    <cellStyle name="Comma 4 5 2 2 5" xfId="197"/>
+    <cellStyle name="Comma 4 5 2 2 6" xfId="198"/>
+    <cellStyle name="Comma 4 5 2 3" xfId="199"/>
+    <cellStyle name="Comma 4 5 2 3 2" xfId="200"/>
+    <cellStyle name="Comma 4 5 2 3 2 2" xfId="201"/>
+    <cellStyle name="Comma 4 5 2 3 3" xfId="202"/>
+    <cellStyle name="Comma 4 5 2 3 4" xfId="203"/>
+    <cellStyle name="Comma 4 5 2 3 5" xfId="204"/>
+    <cellStyle name="Comma 4 5 2 4" xfId="205"/>
+    <cellStyle name="Comma 4 5 2 4 2" xfId="206"/>
+    <cellStyle name="Comma 4 5 2 5" xfId="207"/>
+    <cellStyle name="Comma 4 5 2 6" xfId="208"/>
+    <cellStyle name="Comma 4 5 2 7" xfId="209"/>
+    <cellStyle name="Comma 4 5 3" xfId="210"/>
+    <cellStyle name="Comma 4 5 3 2" xfId="211"/>
+    <cellStyle name="Comma 4 5 3 2 2" xfId="212"/>
+    <cellStyle name="Comma 4 5 3 2 2 2" xfId="213"/>
+    <cellStyle name="Comma 4 5 3 2 3" xfId="214"/>
+    <cellStyle name="Comma 4 5 3 2 4" xfId="215"/>
+    <cellStyle name="Comma 4 5 3 2 5" xfId="216"/>
+    <cellStyle name="Comma 4 5 3 3" xfId="217"/>
+    <cellStyle name="Comma 4 5 3 3 2" xfId="218"/>
+    <cellStyle name="Comma 4 5 3 4" xfId="219"/>
+    <cellStyle name="Comma 4 5 3 5" xfId="220"/>
+    <cellStyle name="Comma 4 5 3 6" xfId="221"/>
+    <cellStyle name="Comma 4 5 4" xfId="222"/>
+    <cellStyle name="Comma 4 5 4 2" xfId="223"/>
+    <cellStyle name="Comma 4 5 4 2 2" xfId="224"/>
+    <cellStyle name="Comma 4 5 4 3" xfId="225"/>
+    <cellStyle name="Comma 4 5 4 4" xfId="226"/>
+    <cellStyle name="Comma 4 5 4 5" xfId="227"/>
+    <cellStyle name="Comma 4 5 5" xfId="228"/>
+    <cellStyle name="Comma 4 5 5 2" xfId="229"/>
+    <cellStyle name="Comma 4 5 6" xfId="230"/>
+    <cellStyle name="Comma 4 5 7" xfId="231"/>
+    <cellStyle name="Comma 4 5 8" xfId="232"/>
+    <cellStyle name="Comma 4 6" xfId="233"/>
+    <cellStyle name="Comma 4 6 2" xfId="234"/>
+    <cellStyle name="Comma 4 6 2 2" xfId="235"/>
+    <cellStyle name="Comma 4 6 2 2 2" xfId="236"/>
+    <cellStyle name="Comma 4 6 2 2 2 2" xfId="237"/>
+    <cellStyle name="Comma 4 6 2 2 3" xfId="238"/>
+    <cellStyle name="Comma 4 6 2 2 4" xfId="239"/>
+    <cellStyle name="Comma 4 6 2 2 5" xfId="240"/>
+    <cellStyle name="Comma 4 6 2 3" xfId="241"/>
+    <cellStyle name="Comma 4 6 2 3 2" xfId="242"/>
+    <cellStyle name="Comma 4 6 2 4" xfId="243"/>
+    <cellStyle name="Comma 4 6 2 5" xfId="244"/>
+    <cellStyle name="Comma 4 6 2 6" xfId="245"/>
+    <cellStyle name="Comma 4 6 3" xfId="246"/>
+    <cellStyle name="Comma 4 6 3 2" xfId="247"/>
+    <cellStyle name="Comma 4 6 3 2 2" xfId="248"/>
+    <cellStyle name="Comma 4 6 3 3" xfId="249"/>
+    <cellStyle name="Comma 4 6 3 4" xfId="250"/>
+    <cellStyle name="Comma 4 6 3 5" xfId="251"/>
+    <cellStyle name="Comma 4 6 4" xfId="252"/>
+    <cellStyle name="Comma 4 6 4 2" xfId="253"/>
+    <cellStyle name="Comma 4 6 5" xfId="254"/>
+    <cellStyle name="Comma 4 6 6" xfId="255"/>
+    <cellStyle name="Comma 4 6 7" xfId="256"/>
+    <cellStyle name="Comma 4 7" xfId="257"/>
+    <cellStyle name="Comma 4 7 2" xfId="258"/>
+    <cellStyle name="Comma 4 7 2 2" xfId="259"/>
+    <cellStyle name="Comma 4 7 2 2 2" xfId="260"/>
+    <cellStyle name="Comma 4 7 2 3" xfId="261"/>
+    <cellStyle name="Comma 4 7 2 4" xfId="262"/>
+    <cellStyle name="Comma 4 7 2 5" xfId="263"/>
+    <cellStyle name="Comma 4 7 3" xfId="264"/>
+    <cellStyle name="Comma 4 7 3 2" xfId="265"/>
+    <cellStyle name="Comma 4 7 4" xfId="266"/>
+    <cellStyle name="Comma 4 7 5" xfId="267"/>
+    <cellStyle name="Comma 4 7 6" xfId="268"/>
+    <cellStyle name="Comma 4 8" xfId="269"/>
+    <cellStyle name="Comma 4 8 2" xfId="270"/>
+    <cellStyle name="Comma 4 8 2 2" xfId="271"/>
+    <cellStyle name="Comma 4 8 3" xfId="272"/>
+    <cellStyle name="Comma 4 8 4" xfId="273"/>
+    <cellStyle name="Comma 4 8 5" xfId="274"/>
+    <cellStyle name="Comma 4 9" xfId="275"/>
+    <cellStyle name="Comma 4 9 2" xfId="276"/>
+    <cellStyle name="Comma 5" xfId="277"/>
+    <cellStyle name="Comma 5 2" xfId="278"/>
+    <cellStyle name="Comma 6" xfId="279"/>
+    <cellStyle name="Comma 7" xfId="280"/>
+    <cellStyle name="Comma 8" xfId="281"/>
+    <cellStyle name="Comma 9" xfId="282"/>
+    <cellStyle name="Currency 2" xfId="283"/>
+    <cellStyle name="Currency 2 2" xfId="284"/>
+    <cellStyle name="Currency 2 3" xfId="285"/>
+    <cellStyle name="Currency 3" xfId="286"/>
+    <cellStyle name="Datatype" xfId="2"/>
+    <cellStyle name="Euro" xfId="287"/>
+    <cellStyle name="Euro 2" xfId="288"/>
+    <cellStyle name="Euro 2 2" xfId="289"/>
     <cellStyle name="Explanatory Text" xfId="883" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text 2" xfId="290" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
-    <cellStyle name="Explanatory Text 2 2" xfId="291" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="290"/>
+    <cellStyle name="Explanatory Text 2 2" xfId="291"/>
     <cellStyle name="Good" xfId="873" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Good 2" xfId="292" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
-    <cellStyle name="Good 2 2" xfId="293" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Good 2" xfId="292"/>
+    <cellStyle name="Good 2 2" xfId="293"/>
     <cellStyle name="Heading 1" xfId="869" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 1 2" xfId="294" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
-    <cellStyle name="Heading 1 2 2" xfId="295" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Heading 1 2" xfId="294"/>
+    <cellStyle name="Heading 1 2 2" xfId="295"/>
     <cellStyle name="Heading 2" xfId="870" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 2 2" xfId="296" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
-    <cellStyle name="Heading 2 2 2" xfId="297" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Heading 2 2" xfId="296"/>
+    <cellStyle name="Heading 2 2 2" xfId="297"/>
     <cellStyle name="Heading 3" xfId="871" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 3 2" xfId="298" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
-    <cellStyle name="Heading 3 2 2" xfId="299" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Heading 3 2" xfId="298"/>
+    <cellStyle name="Heading 3 2 2" xfId="299"/>
     <cellStyle name="Heading 4" xfId="872" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Heading 4 2" xfId="300" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
-    <cellStyle name="Heading 4 2 2" xfId="301" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
-    <cellStyle name="Hyperlink 2" xfId="302" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
-    <cellStyle name="Hyperlink 2 2" xfId="303" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
-    <cellStyle name="Hyperlink 2 3" xfId="304" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
-    <cellStyle name="Hyperlink 2 4" xfId="305" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
-    <cellStyle name="Hyperlink 3" xfId="306" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Heading 4 2" xfId="300"/>
+    <cellStyle name="Heading 4 2 2" xfId="301"/>
+    <cellStyle name="Hyperlink 2" xfId="302"/>
+    <cellStyle name="Hyperlink 2 2" xfId="303"/>
+    <cellStyle name="Hyperlink 2 3" xfId="304"/>
+    <cellStyle name="Hyperlink 2 4" xfId="305"/>
+    <cellStyle name="Hyperlink 3" xfId="306"/>
     <cellStyle name="Input" xfId="876" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Input 2" xfId="307" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
-    <cellStyle name="Input 2 2" xfId="308" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
-    <cellStyle name="Input 2 2 2" xfId="910" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Input 2" xfId="307"/>
+    <cellStyle name="Input 2 2" xfId="308"/>
+    <cellStyle name="Input 2 2 2" xfId="910"/>
     <cellStyle name="Linked Cell" xfId="879" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Linked Cell 2" xfId="309" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
-    <cellStyle name="Linked Cell 2 2" xfId="310" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
-    <cellStyle name="MDYdate" xfId="311" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
-    <cellStyle name="MDYdate 2" xfId="312" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
-    <cellStyle name="MDYdate 2 2" xfId="313" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
-    <cellStyle name="MDYdate 2 3" xfId="314" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Linked Cell 2" xfId="309"/>
+    <cellStyle name="Linked Cell 2 2" xfId="310"/>
+    <cellStyle name="MDYdate" xfId="311"/>
+    <cellStyle name="MDYdate 2" xfId="312"/>
+    <cellStyle name="MDYdate 2 2" xfId="313"/>
+    <cellStyle name="MDYdate 2 3" xfId="314"/>
     <cellStyle name="Neutral" xfId="875" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Neutral 2" xfId="315" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
-    <cellStyle name="Neutral 2 2" xfId="316" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Neutral 2" xfId="315"/>
+    <cellStyle name="Neutral 2 2" xfId="316"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="317" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
-    <cellStyle name="Normal 10 10" xfId="318" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
-    <cellStyle name="Normal 10 2" xfId="319" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
-    <cellStyle name="Normal 10 2 2" xfId="320" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
-    <cellStyle name="Normal 10 2 2 2" xfId="321" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
-    <cellStyle name="Normal 10 2 2 2 2" xfId="322" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
-    <cellStyle name="Normal 10 2 2 2 2 2" xfId="323" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
-    <cellStyle name="Normal 10 2 2 2 3" xfId="324" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
-    <cellStyle name="Normal 10 2 2 2 4" xfId="325" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
-    <cellStyle name="Normal 10 2 2 2 5" xfId="326" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
-    <cellStyle name="Normal 10 2 2 3" xfId="327" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
-    <cellStyle name="Normal 10 2 2 3 2" xfId="328" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
-    <cellStyle name="Normal 10 2 2 4" xfId="329" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
-    <cellStyle name="Normal 10 2 2 5" xfId="330" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
-    <cellStyle name="Normal 10 2 2 6" xfId="331" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
-    <cellStyle name="Normal 10 2 3" xfId="332" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
-    <cellStyle name="Normal 10 2 3 2" xfId="333" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
-    <cellStyle name="Normal 10 2 3 2 2" xfId="334" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
-    <cellStyle name="Normal 10 2 3 3" xfId="335" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
-    <cellStyle name="Normal 10 2 3 4" xfId="336" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
-    <cellStyle name="Normal 10 2 3 5" xfId="337" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
-    <cellStyle name="Normal 10 2 4" xfId="338" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
-    <cellStyle name="Normal 10 2 4 2" xfId="339" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
-    <cellStyle name="Normal 10 2 5" xfId="340" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
-    <cellStyle name="Normal 10 2 6" xfId="341" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
-    <cellStyle name="Normal 10 2 7" xfId="342" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
-    <cellStyle name="Normal 10 3" xfId="343" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
-    <cellStyle name="Normal 10 3 2" xfId="344" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
-    <cellStyle name="Normal 10 3 2 2" xfId="345" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
-    <cellStyle name="Normal 10 3 2 2 2" xfId="346" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
-    <cellStyle name="Normal 10 3 2 3" xfId="347" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
-    <cellStyle name="Normal 10 3 2 4" xfId="348" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
-    <cellStyle name="Normal 10 3 2 5" xfId="349" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
-    <cellStyle name="Normal 10 3 3" xfId="350" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
-    <cellStyle name="Normal 10 3 3 2" xfId="351" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
-    <cellStyle name="Normal 10 3 4" xfId="352" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
-    <cellStyle name="Normal 10 3 5" xfId="353" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
-    <cellStyle name="Normal 10 3 6" xfId="354" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
-    <cellStyle name="Normal 10 4" xfId="355" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
-    <cellStyle name="Normal 10 4 2" xfId="356" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
-    <cellStyle name="Normal 10 4 2 2" xfId="357" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
-    <cellStyle name="Normal 10 4 2 2 2" xfId="358" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
-    <cellStyle name="Normal 10 4 2 3" xfId="359" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
-    <cellStyle name="Normal 10 4 2 4" xfId="360" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
-    <cellStyle name="Normal 10 4 2 5" xfId="361" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
-    <cellStyle name="Normal 10 4 3" xfId="362" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
-    <cellStyle name="Normal 10 4 3 2" xfId="363" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
-    <cellStyle name="Normal 10 4 4" xfId="364" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
-    <cellStyle name="Normal 10 4 5" xfId="365" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
-    <cellStyle name="Normal 10 4 6" xfId="366" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
-    <cellStyle name="Normal 10 5" xfId="367" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
-    <cellStyle name="Normal 10 5 2" xfId="368" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
-    <cellStyle name="Normal 10 5 2 2" xfId="369" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
-    <cellStyle name="Normal 10 5 2 2 2" xfId="370" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
-    <cellStyle name="Normal 10 5 2 3" xfId="371" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
-    <cellStyle name="Normal 10 5 2 4" xfId="372" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
-    <cellStyle name="Normal 10 5 2 5" xfId="373" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
-    <cellStyle name="Normal 10 5 3" xfId="374" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
-    <cellStyle name="Normal 10 5 3 2" xfId="375" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
-    <cellStyle name="Normal 10 5 4" xfId="376" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
-    <cellStyle name="Normal 10 5 5" xfId="377" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
-    <cellStyle name="Normal 10 5 6" xfId="378" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
-    <cellStyle name="Normal 10 6" xfId="379" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
-    <cellStyle name="Normal 10 6 2" xfId="380" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
-    <cellStyle name="Normal 10 6 2 2" xfId="381" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
-    <cellStyle name="Normal 10 6 3" xfId="382" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
-    <cellStyle name="Normal 10 6 4" xfId="383" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
-    <cellStyle name="Normal 10 6 5" xfId="384" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
-    <cellStyle name="Normal 10 7" xfId="385" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
-    <cellStyle name="Normal 10 7 2" xfId="386" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
-    <cellStyle name="Normal 10 8" xfId="387" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
-    <cellStyle name="Normal 10 9" xfId="388" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
-    <cellStyle name="Normal 11" xfId="389" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
-    <cellStyle name="Normal 11 2" xfId="390" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
-    <cellStyle name="Normal 12" xfId="391" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
-    <cellStyle name="Normal 12 2" xfId="392" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
-    <cellStyle name="Normal 13" xfId="393" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
-    <cellStyle name="Normal 13 2" xfId="394" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
-    <cellStyle name="Normal 14" xfId="395" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
-    <cellStyle name="Normal 14 2" xfId="396" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
-    <cellStyle name="Normal 15" xfId="397" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
-    <cellStyle name="Normal 15 2" xfId="398" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
-    <cellStyle name="Normal 151" xfId="914" xr:uid="{69755F86-B1C1-424F-9998-6386918B0332}"/>
-    <cellStyle name="Normal 16" xfId="399" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
-    <cellStyle name="Normal 16 2" xfId="400" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
-    <cellStyle name="Normal 17" xfId="401" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
-    <cellStyle name="Normal 17 2" xfId="402" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
-    <cellStyle name="Normal 17 2 2" xfId="403" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
-    <cellStyle name="Normal 17 3" xfId="404" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
-    <cellStyle name="Normal 18" xfId="405" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
-    <cellStyle name="Normal 18 2" xfId="406" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
-    <cellStyle name="Normal 19" xfId="407" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
-    <cellStyle name="Normal 19 2" xfId="408" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
-    <cellStyle name="Normal 2" xfId="409" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
-    <cellStyle name="Normal 2 2" xfId="410" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="411" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
-    <cellStyle name="Normal 2 2 2 2" xfId="412" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
-    <cellStyle name="Normal 2 2 3" xfId="413" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
-    <cellStyle name="Normal 2 2 3 2" xfId="414" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
-    <cellStyle name="Normal 2 2 4" xfId="415" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
-    <cellStyle name="Normal 2 2 4 2" xfId="416" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
-    <cellStyle name="Normal 2 2 5" xfId="417" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
-    <cellStyle name="Normal 2 3" xfId="418" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
-    <cellStyle name="Normal 2 3 2" xfId="419" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
-    <cellStyle name="Normal 2 3 2 2" xfId="420" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
-    <cellStyle name="Normal 2 3 2 3" xfId="421" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
-    <cellStyle name="Normal 2 3 3" xfId="422" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
-    <cellStyle name="Normal 2 4" xfId="423" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
-    <cellStyle name="Normal 2 4 2" xfId="424" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
-    <cellStyle name="Normal 2 4 3" xfId="425" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
-    <cellStyle name="Normal 2 5" xfId="426" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
-    <cellStyle name="Normal 2 6" xfId="427" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
-    <cellStyle name="Normal 2 6 2" xfId="428" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
-    <cellStyle name="Normal 20" xfId="429" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
-    <cellStyle name="Normal 20 2" xfId="430" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
-    <cellStyle name="Normal 20 2 2" xfId="431" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
-    <cellStyle name="Normal 20 3" xfId="432" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
-    <cellStyle name="Normal 21" xfId="433" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
-    <cellStyle name="Normal 21 2" xfId="434" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
-    <cellStyle name="Normal 22" xfId="435" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
-    <cellStyle name="Normal 22 2" xfId="436" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
-    <cellStyle name="Normal 23" xfId="437" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
-    <cellStyle name="Normal 23 2" xfId="438" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
-    <cellStyle name="Normal 23 2 2" xfId="439" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
-    <cellStyle name="Normal 23 3" xfId="440" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
-    <cellStyle name="Normal 24" xfId="441" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
-    <cellStyle name="Normal 24 2" xfId="442" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
-    <cellStyle name="Normal 25" xfId="443" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
-    <cellStyle name="Normal 25 2" xfId="444" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
-    <cellStyle name="Normal 26" xfId="445" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
-    <cellStyle name="Normal 26 2" xfId="446" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
-    <cellStyle name="Normal 27" xfId="447" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
-    <cellStyle name="Normal 27 2" xfId="448" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
-    <cellStyle name="Normal 28" xfId="449" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
-    <cellStyle name="Normal 28 2" xfId="450" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
-    <cellStyle name="Normal 29" xfId="451" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
-    <cellStyle name="Normal 29 2" xfId="452" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
-    <cellStyle name="Normal 3 2" xfId="453" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="454" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="455" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
-    <cellStyle name="Normal 3 2 4" xfId="456" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
-    <cellStyle name="Normal 3 2 5" xfId="457" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
-    <cellStyle name="Normal 3 2 6" xfId="458" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
-    <cellStyle name="Normal 3 3" xfId="459" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="460" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="461" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
-    <cellStyle name="Normal 3 4" xfId="462" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
-    <cellStyle name="Normal 3 5" xfId="463" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
-    <cellStyle name="Normal 3 6" xfId="464" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
-    <cellStyle name="Normal 3 6 2" xfId="465" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
-    <cellStyle name="Normal 3 6 3" xfId="466" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
-    <cellStyle name="Normal 3 7" xfId="467" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
-    <cellStyle name="Normal 3 8" xfId="468" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
-    <cellStyle name="Normal 30" xfId="469" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
-    <cellStyle name="Normal 30 2" xfId="470" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
-    <cellStyle name="Normal 31" xfId="471" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
-    <cellStyle name="Normal 31 2" xfId="472" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
-    <cellStyle name="Normal 32" xfId="473" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
-    <cellStyle name="Normal 32 2" xfId="474" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
-    <cellStyle name="Normal 33" xfId="475" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
-    <cellStyle name="Normal 33 2" xfId="476" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
-    <cellStyle name="Normal 34" xfId="477" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
-    <cellStyle name="Normal 34 2" xfId="478" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
-    <cellStyle name="Normal 35" xfId="479" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
-    <cellStyle name="Normal 35 2" xfId="480" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
-    <cellStyle name="Normal 36" xfId="481" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
-    <cellStyle name="Normal 36 2" xfId="482" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
-    <cellStyle name="Normal 37" xfId="483" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
-    <cellStyle name="Normal 37 2" xfId="484" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
-    <cellStyle name="Normal 37 2 2" xfId="485" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
-    <cellStyle name="Normal 37 3" xfId="486" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
-    <cellStyle name="Normal 37 4" xfId="487" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
-    <cellStyle name="Normal 37 5" xfId="488" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
-    <cellStyle name="Normal 38" xfId="489" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
-    <cellStyle name="Normal 38 2" xfId="490" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
-    <cellStyle name="Normal 39" xfId="491" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
-    <cellStyle name="Normal 39 2" xfId="492" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
-    <cellStyle name="Normal 39 2 2" xfId="493" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
-    <cellStyle name="Normal 39 3" xfId="494" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
-    <cellStyle name="Normal 4" xfId="495" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
-    <cellStyle name="Normal 4 2" xfId="496" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
-    <cellStyle name="Normal 4 3" xfId="497" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
-    <cellStyle name="Normal 4 3 2" xfId="498" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
-    <cellStyle name="Normal 4 4" xfId="499" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
-    <cellStyle name="Normal 40" xfId="500" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
-    <cellStyle name="Normal 40 2" xfId="501" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
-    <cellStyle name="Normal 41" xfId="502" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
-    <cellStyle name="Normal 41 2" xfId="503" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
-    <cellStyle name="Normal 42" xfId="504" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
-    <cellStyle name="Normal 42 2" xfId="505" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
-    <cellStyle name="Normal 43" xfId="506" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
-    <cellStyle name="Normal 43 2" xfId="507" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
-    <cellStyle name="Normal 44" xfId="508" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
-    <cellStyle name="Normal 44 2" xfId="509" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
-    <cellStyle name="Normal 45" xfId="510" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
-    <cellStyle name="Normal 45 2" xfId="511" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
-    <cellStyle name="Normal 46" xfId="512" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
-    <cellStyle name="Normal 46 2" xfId="513" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
-    <cellStyle name="Normal 47" xfId="514" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
-    <cellStyle name="Normal 47 2" xfId="515" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
-    <cellStyle name="Normal 48" xfId="516" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
-    <cellStyle name="Normal 48 2" xfId="517" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
-    <cellStyle name="Normal 49" xfId="518" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
-    <cellStyle name="Normal 49 2" xfId="519" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
-    <cellStyle name="Normal 5" xfId="520" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
-    <cellStyle name="Normal 5 2" xfId="521" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
-    <cellStyle name="Normal 5 3" xfId="522" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
-    <cellStyle name="Normal 5 3 2" xfId="523" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
-    <cellStyle name="Normal 5 4" xfId="524" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
-    <cellStyle name="Normal 50" xfId="525" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
-    <cellStyle name="Normal 50 2" xfId="526" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
-    <cellStyle name="Normal 51" xfId="527" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
-    <cellStyle name="Normal 51 2" xfId="528" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
-    <cellStyle name="Normal 52" xfId="529" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
-    <cellStyle name="Normal 52 2" xfId="530" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
-    <cellStyle name="Normal 53" xfId="531" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
-    <cellStyle name="Normal 53 2" xfId="532" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
-    <cellStyle name="Normal 54" xfId="533" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
-    <cellStyle name="Normal 54 2" xfId="534" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
-    <cellStyle name="Normal 55" xfId="535" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
-    <cellStyle name="Normal 56" xfId="536" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
-    <cellStyle name="Normal 6" xfId="537" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
-    <cellStyle name="Normal 6 10" xfId="538" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
-    <cellStyle name="Normal 6 11" xfId="539" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
-    <cellStyle name="Normal 6 12" xfId="540" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
-    <cellStyle name="Normal 6 2" xfId="541" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
-    <cellStyle name="Normal 6 2 2" xfId="542" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
-    <cellStyle name="Normal 6 2 3" xfId="543" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
-    <cellStyle name="Normal 6 3" xfId="544" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
-    <cellStyle name="Normal 6 4" xfId="545" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
-    <cellStyle name="Normal 6 4 2" xfId="546" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="547" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
-    <cellStyle name="Normal 6 4 2 2 2" xfId="548" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 2" xfId="549" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="550" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 3" xfId="551" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 4" xfId="552" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 5" xfId="553" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
-    <cellStyle name="Normal 6 4 2 2 3" xfId="554" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 2" xfId="555" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
-    <cellStyle name="Normal 6 4 2 2 4" xfId="556" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
-    <cellStyle name="Normal 6 4 2 2 5" xfId="557" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
-    <cellStyle name="Normal 6 4 2 2 6" xfId="558" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
-    <cellStyle name="Normal 6 4 2 3" xfId="559" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
-    <cellStyle name="Normal 6 4 2 3 2" xfId="560" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
-    <cellStyle name="Normal 6 4 2 3 2 2" xfId="561" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
-    <cellStyle name="Normal 6 4 2 3 3" xfId="562" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
-    <cellStyle name="Normal 6 4 2 3 4" xfId="563" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
-    <cellStyle name="Normal 6 4 2 3 5" xfId="564" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
-    <cellStyle name="Normal 6 4 2 4" xfId="565" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
-    <cellStyle name="Normal 6 4 2 4 2" xfId="566" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
-    <cellStyle name="Normal 6 4 2 5" xfId="567" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
-    <cellStyle name="Normal 6 4 2 6" xfId="568" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
-    <cellStyle name="Normal 6 4 2 7" xfId="569" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
-    <cellStyle name="Normal 6 4 3" xfId="570" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
-    <cellStyle name="Normal 6 4 3 2" xfId="571" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
-    <cellStyle name="Normal 6 4 3 2 2" xfId="572" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
-    <cellStyle name="Normal 6 4 3 2 2 2" xfId="573" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
-    <cellStyle name="Normal 6 4 3 2 3" xfId="574" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
-    <cellStyle name="Normal 6 4 3 2 4" xfId="575" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
-    <cellStyle name="Normal 6 4 3 2 5" xfId="576" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
-    <cellStyle name="Normal 6 4 3 3" xfId="577" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
-    <cellStyle name="Normal 6 4 3 3 2" xfId="578" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
-    <cellStyle name="Normal 6 4 3 4" xfId="579" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
-    <cellStyle name="Normal 6 4 3 5" xfId="580" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
-    <cellStyle name="Normal 6 4 3 6" xfId="581" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
-    <cellStyle name="Normal 6 4 4" xfId="582" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
-    <cellStyle name="Normal 6 4 4 2" xfId="583" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
-    <cellStyle name="Normal 6 4 4 2 2" xfId="584" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
-    <cellStyle name="Normal 6 4 4 3" xfId="585" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
-    <cellStyle name="Normal 6 4 4 4" xfId="586" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
-    <cellStyle name="Normal 6 4 4 5" xfId="587" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
-    <cellStyle name="Normal 6 4 5" xfId="588" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
-    <cellStyle name="Normal 6 4 5 2" xfId="589" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
-    <cellStyle name="Normal 6 4 6" xfId="590" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
-    <cellStyle name="Normal 6 4 7" xfId="591" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
-    <cellStyle name="Normal 6 4 8" xfId="592" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
-    <cellStyle name="Normal 6 5" xfId="593" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
-    <cellStyle name="Normal 6 5 2" xfId="594" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="595" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
-    <cellStyle name="Normal 6 5 2 2 2" xfId="596" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 2" xfId="597" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
-    <cellStyle name="Normal 6 5 2 2 3" xfId="598" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
-    <cellStyle name="Normal 6 5 2 2 4" xfId="599" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
-    <cellStyle name="Normal 6 5 2 2 5" xfId="600" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
-    <cellStyle name="Normal 6 5 2 3" xfId="601" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
-    <cellStyle name="Normal 6 5 2 3 2" xfId="602" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
-    <cellStyle name="Normal 6 5 2 4" xfId="603" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
-    <cellStyle name="Normal 6 5 2 5" xfId="604" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
-    <cellStyle name="Normal 6 5 2 6" xfId="605" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
-    <cellStyle name="Normal 6 5 3" xfId="606" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
-    <cellStyle name="Normal 6 5 3 2" xfId="607" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
-    <cellStyle name="Normal 6 5 3 2 2" xfId="608" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
-    <cellStyle name="Normal 6 5 3 3" xfId="609" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
-    <cellStyle name="Normal 6 5 3 4" xfId="610" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
-    <cellStyle name="Normal 6 5 3 5" xfId="611" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
-    <cellStyle name="Normal 6 5 4" xfId="612" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
-    <cellStyle name="Normal 6 5 4 2" xfId="613" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
-    <cellStyle name="Normal 6 5 5" xfId="614" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
-    <cellStyle name="Normal 6 5 6" xfId="615" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
-    <cellStyle name="Normal 6 5 7" xfId="616" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
-    <cellStyle name="Normal 6 6" xfId="617" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
-    <cellStyle name="Normal 6 6 2" xfId="618" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
-    <cellStyle name="Normal 6 6 2 2" xfId="619" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
-    <cellStyle name="Normal 6 6 2 2 2" xfId="620" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
-    <cellStyle name="Normal 6 6 2 3" xfId="621" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
-    <cellStyle name="Normal 6 6 2 4" xfId="622" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
-    <cellStyle name="Normal 6 6 2 5" xfId="623" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
-    <cellStyle name="Normal 6 6 3" xfId="624" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
-    <cellStyle name="Normal 6 6 3 2" xfId="625" xr:uid="{00000000-0005-0000-0000-000097020000}"/>
-    <cellStyle name="Normal 6 6 4" xfId="626" xr:uid="{00000000-0005-0000-0000-000098020000}"/>
-    <cellStyle name="Normal 6 6 5" xfId="627" xr:uid="{00000000-0005-0000-0000-000099020000}"/>
-    <cellStyle name="Normal 6 6 6" xfId="628" xr:uid="{00000000-0005-0000-0000-00009A020000}"/>
-    <cellStyle name="Normal 6 7" xfId="629" xr:uid="{00000000-0005-0000-0000-00009B020000}"/>
-    <cellStyle name="Normal 6 7 2" xfId="630" xr:uid="{00000000-0005-0000-0000-00009C020000}"/>
-    <cellStyle name="Normal 6 7 2 2" xfId="631" xr:uid="{00000000-0005-0000-0000-00009D020000}"/>
-    <cellStyle name="Normal 6 7 3" xfId="632" xr:uid="{00000000-0005-0000-0000-00009E020000}"/>
-    <cellStyle name="Normal 6 7 4" xfId="633" xr:uid="{00000000-0005-0000-0000-00009F020000}"/>
-    <cellStyle name="Normal 6 7 5" xfId="634" xr:uid="{00000000-0005-0000-0000-0000A0020000}"/>
-    <cellStyle name="Normal 6 8" xfId="635" xr:uid="{00000000-0005-0000-0000-0000A1020000}"/>
-    <cellStyle name="Normal 6 9" xfId="636" xr:uid="{00000000-0005-0000-0000-0000A2020000}"/>
-    <cellStyle name="Normal 6 9 2" xfId="637" xr:uid="{00000000-0005-0000-0000-0000A3020000}"/>
-    <cellStyle name="Normal 7" xfId="638" xr:uid="{00000000-0005-0000-0000-0000A4020000}"/>
-    <cellStyle name="Normal 7 10" xfId="639" xr:uid="{00000000-0005-0000-0000-0000A5020000}"/>
-    <cellStyle name="Normal 7 11" xfId="640" xr:uid="{00000000-0005-0000-0000-0000A6020000}"/>
-    <cellStyle name="Normal 7 2" xfId="641" xr:uid="{00000000-0005-0000-0000-0000A7020000}"/>
-    <cellStyle name="Normal 7 2 2" xfId="642" xr:uid="{00000000-0005-0000-0000-0000A8020000}"/>
-    <cellStyle name="Normal 7 3" xfId="643" xr:uid="{00000000-0005-0000-0000-0000A9020000}"/>
-    <cellStyle name="Normal 7 3 2" xfId="644" xr:uid="{00000000-0005-0000-0000-0000AA020000}"/>
-    <cellStyle name="Normal 7 4" xfId="645" xr:uid="{00000000-0005-0000-0000-0000AB020000}"/>
-    <cellStyle name="Normal 7 4 2" xfId="646" xr:uid="{00000000-0005-0000-0000-0000AC020000}"/>
-    <cellStyle name="Normal 7 4 2 2" xfId="647" xr:uid="{00000000-0005-0000-0000-0000AD020000}"/>
-    <cellStyle name="Normal 7 4 2 2 2" xfId="648" xr:uid="{00000000-0005-0000-0000-0000AE020000}"/>
-    <cellStyle name="Normal 7 4 2 2 2 2" xfId="649" xr:uid="{00000000-0005-0000-0000-0000AF020000}"/>
-    <cellStyle name="Normal 7 4 2 2 2 2 2" xfId="650" xr:uid="{00000000-0005-0000-0000-0000B0020000}"/>
-    <cellStyle name="Normal 7 4 2 2 2 3" xfId="651" xr:uid="{00000000-0005-0000-0000-0000B1020000}"/>
-    <cellStyle name="Normal 7 4 2 2 2 4" xfId="652" xr:uid="{00000000-0005-0000-0000-0000B2020000}"/>
-    <cellStyle name="Normal 7 4 2 2 2 5" xfId="653" xr:uid="{00000000-0005-0000-0000-0000B3020000}"/>
-    <cellStyle name="Normal 7 4 2 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-0000B4020000}"/>
-    <cellStyle name="Normal 7 4 2 2 3 2" xfId="655" xr:uid="{00000000-0005-0000-0000-0000B5020000}"/>
-    <cellStyle name="Normal 7 4 2 2 4" xfId="656" xr:uid="{00000000-0005-0000-0000-0000B6020000}"/>
-    <cellStyle name="Normal 7 4 2 2 5" xfId="657" xr:uid="{00000000-0005-0000-0000-0000B7020000}"/>
-    <cellStyle name="Normal 7 4 2 2 6" xfId="658" xr:uid="{00000000-0005-0000-0000-0000B8020000}"/>
-    <cellStyle name="Normal 7 4 2 3" xfId="659" xr:uid="{00000000-0005-0000-0000-0000B9020000}"/>
-    <cellStyle name="Normal 7 4 2 3 2" xfId="660" xr:uid="{00000000-0005-0000-0000-0000BA020000}"/>
-    <cellStyle name="Normal 7 4 2 3 2 2" xfId="661" xr:uid="{00000000-0005-0000-0000-0000BB020000}"/>
-    <cellStyle name="Normal 7 4 2 3 3" xfId="662" xr:uid="{00000000-0005-0000-0000-0000BC020000}"/>
-    <cellStyle name="Normal 7 4 2 3 4" xfId="663" xr:uid="{00000000-0005-0000-0000-0000BD020000}"/>
-    <cellStyle name="Normal 7 4 2 3 5" xfId="664" xr:uid="{00000000-0005-0000-0000-0000BE020000}"/>
-    <cellStyle name="Normal 7 4 2 4" xfId="665" xr:uid="{00000000-0005-0000-0000-0000BF020000}"/>
-    <cellStyle name="Normal 7 4 2 4 2" xfId="666" xr:uid="{00000000-0005-0000-0000-0000C0020000}"/>
-    <cellStyle name="Normal 7 4 2 5" xfId="667" xr:uid="{00000000-0005-0000-0000-0000C1020000}"/>
-    <cellStyle name="Normal 7 4 2 6" xfId="668" xr:uid="{00000000-0005-0000-0000-0000C2020000}"/>
-    <cellStyle name="Normal 7 4 2 7" xfId="669" xr:uid="{00000000-0005-0000-0000-0000C3020000}"/>
-    <cellStyle name="Normal 7 4 3" xfId="670" xr:uid="{00000000-0005-0000-0000-0000C4020000}"/>
-    <cellStyle name="Normal 7 4 3 2" xfId="671" xr:uid="{00000000-0005-0000-0000-0000C5020000}"/>
-    <cellStyle name="Normal 7 4 3 2 2" xfId="672" xr:uid="{00000000-0005-0000-0000-0000C6020000}"/>
-    <cellStyle name="Normal 7 4 3 2 2 2" xfId="673" xr:uid="{00000000-0005-0000-0000-0000C7020000}"/>
-    <cellStyle name="Normal 7 4 3 2 3" xfId="674" xr:uid="{00000000-0005-0000-0000-0000C8020000}"/>
-    <cellStyle name="Normal 7 4 3 2 4" xfId="675" xr:uid="{00000000-0005-0000-0000-0000C9020000}"/>
-    <cellStyle name="Normal 7 4 3 2 5" xfId="676" xr:uid="{00000000-0005-0000-0000-0000CA020000}"/>
-    <cellStyle name="Normal 7 4 3 3" xfId="677" xr:uid="{00000000-0005-0000-0000-0000CB020000}"/>
-    <cellStyle name="Normal 7 4 3 3 2" xfId="678" xr:uid="{00000000-0005-0000-0000-0000CC020000}"/>
-    <cellStyle name="Normal 7 4 3 4" xfId="679" xr:uid="{00000000-0005-0000-0000-0000CD020000}"/>
-    <cellStyle name="Normal 7 4 3 5" xfId="680" xr:uid="{00000000-0005-0000-0000-0000CE020000}"/>
-    <cellStyle name="Normal 7 4 3 6" xfId="681" xr:uid="{00000000-0005-0000-0000-0000CF020000}"/>
-    <cellStyle name="Normal 7 4 4" xfId="682" xr:uid="{00000000-0005-0000-0000-0000D0020000}"/>
-    <cellStyle name="Normal 7 4 4 2" xfId="683" xr:uid="{00000000-0005-0000-0000-0000D1020000}"/>
-    <cellStyle name="Normal 7 4 4 2 2" xfId="684" xr:uid="{00000000-0005-0000-0000-0000D2020000}"/>
-    <cellStyle name="Normal 7 4 4 3" xfId="685" xr:uid="{00000000-0005-0000-0000-0000D3020000}"/>
-    <cellStyle name="Normal 7 4 4 4" xfId="686" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
-    <cellStyle name="Normal 7 4 4 5" xfId="687" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
-    <cellStyle name="Normal 7 4 5" xfId="688" xr:uid="{00000000-0005-0000-0000-0000D6020000}"/>
-    <cellStyle name="Normal 7 4 5 2" xfId="689" xr:uid="{00000000-0005-0000-0000-0000D7020000}"/>
-    <cellStyle name="Normal 7 4 6" xfId="690" xr:uid="{00000000-0005-0000-0000-0000D8020000}"/>
-    <cellStyle name="Normal 7 4 7" xfId="691" xr:uid="{00000000-0005-0000-0000-0000D9020000}"/>
-    <cellStyle name="Normal 7 4 8" xfId="692" xr:uid="{00000000-0005-0000-0000-0000DA020000}"/>
-    <cellStyle name="Normal 7 5" xfId="693" xr:uid="{00000000-0005-0000-0000-0000DB020000}"/>
-    <cellStyle name="Normal 7 5 2" xfId="694" xr:uid="{00000000-0005-0000-0000-0000DC020000}"/>
-    <cellStyle name="Normal 7 5 2 2" xfId="695" xr:uid="{00000000-0005-0000-0000-0000DD020000}"/>
-    <cellStyle name="Normal 7 5 2 2 2" xfId="696" xr:uid="{00000000-0005-0000-0000-0000DE020000}"/>
-    <cellStyle name="Normal 7 5 2 2 2 2" xfId="697" xr:uid="{00000000-0005-0000-0000-0000DF020000}"/>
-    <cellStyle name="Normal 7 5 2 2 3" xfId="698" xr:uid="{00000000-0005-0000-0000-0000E0020000}"/>
-    <cellStyle name="Normal 7 5 2 2 4" xfId="699" xr:uid="{00000000-0005-0000-0000-0000E1020000}"/>
-    <cellStyle name="Normal 7 5 2 2 5" xfId="700" xr:uid="{00000000-0005-0000-0000-0000E2020000}"/>
-    <cellStyle name="Normal 7 5 2 3" xfId="701" xr:uid="{00000000-0005-0000-0000-0000E3020000}"/>
-    <cellStyle name="Normal 7 5 2 3 2" xfId="702" xr:uid="{00000000-0005-0000-0000-0000E4020000}"/>
-    <cellStyle name="Normal 7 5 2 4" xfId="703" xr:uid="{00000000-0005-0000-0000-0000E5020000}"/>
-    <cellStyle name="Normal 7 5 2 5" xfId="704" xr:uid="{00000000-0005-0000-0000-0000E6020000}"/>
-    <cellStyle name="Normal 7 5 2 6" xfId="705" xr:uid="{00000000-0005-0000-0000-0000E7020000}"/>
-    <cellStyle name="Normal 7 5 3" xfId="706" xr:uid="{00000000-0005-0000-0000-0000E8020000}"/>
-    <cellStyle name="Normal 7 5 3 2" xfId="707" xr:uid="{00000000-0005-0000-0000-0000E9020000}"/>
-    <cellStyle name="Normal 7 5 3 2 2" xfId="708" xr:uid="{00000000-0005-0000-0000-0000EA020000}"/>
-    <cellStyle name="Normal 7 5 3 3" xfId="709" xr:uid="{00000000-0005-0000-0000-0000EB020000}"/>
-    <cellStyle name="Normal 7 5 3 4" xfId="710" xr:uid="{00000000-0005-0000-0000-0000EC020000}"/>
-    <cellStyle name="Normal 7 5 3 5" xfId="711" xr:uid="{00000000-0005-0000-0000-0000ED020000}"/>
-    <cellStyle name="Normal 7 5 4" xfId="712" xr:uid="{00000000-0005-0000-0000-0000EE020000}"/>
-    <cellStyle name="Normal 7 5 4 2" xfId="713" xr:uid="{00000000-0005-0000-0000-0000EF020000}"/>
-    <cellStyle name="Normal 7 5 5" xfId="714" xr:uid="{00000000-0005-0000-0000-0000F0020000}"/>
-    <cellStyle name="Normal 7 5 6" xfId="715" xr:uid="{00000000-0005-0000-0000-0000F1020000}"/>
-    <cellStyle name="Normal 7 5 7" xfId="716" xr:uid="{00000000-0005-0000-0000-0000F2020000}"/>
-    <cellStyle name="Normal 7 6" xfId="717" xr:uid="{00000000-0005-0000-0000-0000F3020000}"/>
-    <cellStyle name="Normal 7 6 2" xfId="718" xr:uid="{00000000-0005-0000-0000-0000F4020000}"/>
-    <cellStyle name="Normal 7 6 2 2" xfId="719" xr:uid="{00000000-0005-0000-0000-0000F5020000}"/>
-    <cellStyle name="Normal 7 6 2 2 2" xfId="720" xr:uid="{00000000-0005-0000-0000-0000F6020000}"/>
-    <cellStyle name="Normal 7 6 2 3" xfId="721" xr:uid="{00000000-0005-0000-0000-0000F7020000}"/>
-    <cellStyle name="Normal 7 6 2 4" xfId="722" xr:uid="{00000000-0005-0000-0000-0000F8020000}"/>
-    <cellStyle name="Normal 7 6 2 5" xfId="723" xr:uid="{00000000-0005-0000-0000-0000F9020000}"/>
-    <cellStyle name="Normal 7 6 3" xfId="724" xr:uid="{00000000-0005-0000-0000-0000FA020000}"/>
-    <cellStyle name="Normal 7 6 3 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000FB020000}"/>
-    <cellStyle name="Normal 7 6 4" xfId="726" xr:uid="{00000000-0005-0000-0000-0000FC020000}"/>
-    <cellStyle name="Normal 7 6 5" xfId="727" xr:uid="{00000000-0005-0000-0000-0000FD020000}"/>
-    <cellStyle name="Normal 7 6 6" xfId="728" xr:uid="{00000000-0005-0000-0000-0000FE020000}"/>
-    <cellStyle name="Normal 7 7" xfId="729" xr:uid="{00000000-0005-0000-0000-0000FF020000}"/>
-    <cellStyle name="Normal 7 7 2" xfId="730" xr:uid="{00000000-0005-0000-0000-000000030000}"/>
-    <cellStyle name="Normal 7 7 2 2" xfId="731" xr:uid="{00000000-0005-0000-0000-000001030000}"/>
-    <cellStyle name="Normal 7 7 3" xfId="732" xr:uid="{00000000-0005-0000-0000-000002030000}"/>
-    <cellStyle name="Normal 7 7 4" xfId="733" xr:uid="{00000000-0005-0000-0000-000003030000}"/>
-    <cellStyle name="Normal 7 7 5" xfId="734" xr:uid="{00000000-0005-0000-0000-000004030000}"/>
-    <cellStyle name="Normal 7 8" xfId="735" xr:uid="{00000000-0005-0000-0000-000005030000}"/>
-    <cellStyle name="Normal 7 8 2" xfId="736" xr:uid="{00000000-0005-0000-0000-000006030000}"/>
-    <cellStyle name="Normal 7 9" xfId="737" xr:uid="{00000000-0005-0000-0000-000007030000}"/>
-    <cellStyle name="Normal 8" xfId="738" xr:uid="{00000000-0005-0000-0000-000008030000}"/>
-    <cellStyle name="Normal 8 2" xfId="739" xr:uid="{00000000-0005-0000-0000-000009030000}"/>
-    <cellStyle name="Normal 9" xfId="740" xr:uid="{00000000-0005-0000-0000-00000A030000}"/>
-    <cellStyle name="Normal 9 2" xfId="741" xr:uid="{00000000-0005-0000-0000-00000B030000}"/>
+    <cellStyle name="Normal 10" xfId="317"/>
+    <cellStyle name="Normal 10 10" xfId="318"/>
+    <cellStyle name="Normal 10 2" xfId="319"/>
+    <cellStyle name="Normal 10 2 2" xfId="320"/>
+    <cellStyle name="Normal 10 2 2 2" xfId="321"/>
+    <cellStyle name="Normal 10 2 2 2 2" xfId="322"/>
+    <cellStyle name="Normal 10 2 2 2 2 2" xfId="323"/>
+    <cellStyle name="Normal 10 2 2 2 3" xfId="324"/>
+    <cellStyle name="Normal 10 2 2 2 4" xfId="325"/>
+    <cellStyle name="Normal 10 2 2 2 5" xfId="326"/>
+    <cellStyle name="Normal 10 2 2 3" xfId="327"/>
+    <cellStyle name="Normal 10 2 2 3 2" xfId="328"/>
+    <cellStyle name="Normal 10 2 2 4" xfId="329"/>
+    <cellStyle name="Normal 10 2 2 5" xfId="330"/>
+    <cellStyle name="Normal 10 2 2 6" xfId="331"/>
+    <cellStyle name="Normal 10 2 3" xfId="332"/>
+    <cellStyle name="Normal 10 2 3 2" xfId="333"/>
+    <cellStyle name="Normal 10 2 3 2 2" xfId="334"/>
+    <cellStyle name="Normal 10 2 3 3" xfId="335"/>
+    <cellStyle name="Normal 10 2 3 4" xfId="336"/>
+    <cellStyle name="Normal 10 2 3 5" xfId="337"/>
+    <cellStyle name="Normal 10 2 4" xfId="338"/>
+    <cellStyle name="Normal 10 2 4 2" xfId="339"/>
+    <cellStyle name="Normal 10 2 5" xfId="340"/>
+    <cellStyle name="Normal 10 2 6" xfId="341"/>
+    <cellStyle name="Normal 10 2 7" xfId="342"/>
+    <cellStyle name="Normal 10 3" xfId="343"/>
+    <cellStyle name="Normal 10 3 2" xfId="344"/>
+    <cellStyle name="Normal 10 3 2 2" xfId="345"/>
+    <cellStyle name="Normal 10 3 2 2 2" xfId="346"/>
+    <cellStyle name="Normal 10 3 2 3" xfId="347"/>
+    <cellStyle name="Normal 10 3 2 4" xfId="348"/>
+    <cellStyle name="Normal 10 3 2 5" xfId="349"/>
+    <cellStyle name="Normal 10 3 3" xfId="350"/>
+    <cellStyle name="Normal 10 3 3 2" xfId="351"/>
+    <cellStyle name="Normal 10 3 4" xfId="352"/>
+    <cellStyle name="Normal 10 3 5" xfId="353"/>
+    <cellStyle name="Normal 10 3 6" xfId="354"/>
+    <cellStyle name="Normal 10 4" xfId="355"/>
+    <cellStyle name="Normal 10 4 2" xfId="356"/>
+    <cellStyle name="Normal 10 4 2 2" xfId="357"/>
+    <cellStyle name="Normal 10 4 2 2 2" xfId="358"/>
+    <cellStyle name="Normal 10 4 2 3" xfId="359"/>
+    <cellStyle name="Normal 10 4 2 4" xfId="360"/>
+    <cellStyle name="Normal 10 4 2 5" xfId="361"/>
+    <cellStyle name="Normal 10 4 3" xfId="362"/>
+    <cellStyle name="Normal 10 4 3 2" xfId="363"/>
+    <cellStyle name="Normal 10 4 4" xfId="364"/>
+    <cellStyle name="Normal 10 4 5" xfId="365"/>
+    <cellStyle name="Normal 10 4 6" xfId="366"/>
+    <cellStyle name="Normal 10 5" xfId="367"/>
+    <cellStyle name="Normal 10 5 2" xfId="368"/>
+    <cellStyle name="Normal 10 5 2 2" xfId="369"/>
+    <cellStyle name="Normal 10 5 2 2 2" xfId="370"/>
+    <cellStyle name="Normal 10 5 2 3" xfId="371"/>
+    <cellStyle name="Normal 10 5 2 4" xfId="372"/>
+    <cellStyle name="Normal 10 5 2 5" xfId="373"/>
+    <cellStyle name="Normal 10 5 3" xfId="374"/>
+    <cellStyle name="Normal 10 5 3 2" xfId="375"/>
+    <cellStyle name="Normal 10 5 4" xfId="376"/>
+    <cellStyle name="Normal 10 5 5" xfId="377"/>
+    <cellStyle name="Normal 10 5 6" xfId="378"/>
+    <cellStyle name="Normal 10 6" xfId="379"/>
+    <cellStyle name="Normal 10 6 2" xfId="380"/>
+    <cellStyle name="Normal 10 6 2 2" xfId="381"/>
+    <cellStyle name="Normal 10 6 3" xfId="382"/>
+    <cellStyle name="Normal 10 6 4" xfId="383"/>
+    <cellStyle name="Normal 10 6 5" xfId="384"/>
+    <cellStyle name="Normal 10 7" xfId="385"/>
+    <cellStyle name="Normal 10 7 2" xfId="386"/>
+    <cellStyle name="Normal 10 8" xfId="387"/>
+    <cellStyle name="Normal 10 9" xfId="388"/>
+    <cellStyle name="Normal 11" xfId="389"/>
+    <cellStyle name="Normal 11 2" xfId="390"/>
+    <cellStyle name="Normal 12" xfId="391"/>
+    <cellStyle name="Normal 12 2" xfId="392"/>
+    <cellStyle name="Normal 13" xfId="393"/>
+    <cellStyle name="Normal 13 2" xfId="394"/>
+    <cellStyle name="Normal 14" xfId="395"/>
+    <cellStyle name="Normal 14 2" xfId="396"/>
+    <cellStyle name="Normal 15" xfId="397"/>
+    <cellStyle name="Normal 15 2" xfId="398"/>
+    <cellStyle name="Normal 151" xfId="914"/>
+    <cellStyle name="Normal 16" xfId="399"/>
+    <cellStyle name="Normal 16 2" xfId="400"/>
+    <cellStyle name="Normal 17" xfId="401"/>
+    <cellStyle name="Normal 17 2" xfId="402"/>
+    <cellStyle name="Normal 17 2 2" xfId="403"/>
+    <cellStyle name="Normal 17 3" xfId="404"/>
+    <cellStyle name="Normal 18" xfId="405"/>
+    <cellStyle name="Normal 18 2" xfId="406"/>
+    <cellStyle name="Normal 19" xfId="407"/>
+    <cellStyle name="Normal 19 2" xfId="408"/>
+    <cellStyle name="Normal 2" xfId="409"/>
+    <cellStyle name="Normal 2 2" xfId="410"/>
+    <cellStyle name="Normal 2 2 2" xfId="411"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="412"/>
+    <cellStyle name="Normal 2 2 3" xfId="413"/>
+    <cellStyle name="Normal 2 2 3 2" xfId="414"/>
+    <cellStyle name="Normal 2 2 4" xfId="415"/>
+    <cellStyle name="Normal 2 2 4 2" xfId="416"/>
+    <cellStyle name="Normal 2 2 5" xfId="417"/>
+    <cellStyle name="Normal 2 3" xfId="418"/>
+    <cellStyle name="Normal 2 3 2" xfId="419"/>
+    <cellStyle name="Normal 2 3 2 2" xfId="420"/>
+    <cellStyle name="Normal 2 3 2 3" xfId="421"/>
+    <cellStyle name="Normal 2 3 3" xfId="422"/>
+    <cellStyle name="Normal 2 4" xfId="423"/>
+    <cellStyle name="Normal 2 4 2" xfId="424"/>
+    <cellStyle name="Normal 2 4 3" xfId="425"/>
+    <cellStyle name="Normal 2 5" xfId="426"/>
+    <cellStyle name="Normal 2 6" xfId="427"/>
+    <cellStyle name="Normal 2 6 2" xfId="428"/>
+    <cellStyle name="Normal 20" xfId="429"/>
+    <cellStyle name="Normal 20 2" xfId="430"/>
+    <cellStyle name="Normal 20 2 2" xfId="431"/>
+    <cellStyle name="Normal 20 3" xfId="432"/>
+    <cellStyle name="Normal 21" xfId="433"/>
+    <cellStyle name="Normal 21 2" xfId="434"/>
+    <cellStyle name="Normal 22" xfId="435"/>
+    <cellStyle name="Normal 22 2" xfId="436"/>
+    <cellStyle name="Normal 23" xfId="437"/>
+    <cellStyle name="Normal 23 2" xfId="438"/>
+    <cellStyle name="Normal 23 2 2" xfId="439"/>
+    <cellStyle name="Normal 23 3" xfId="440"/>
+    <cellStyle name="Normal 24" xfId="441"/>
+    <cellStyle name="Normal 24 2" xfId="442"/>
+    <cellStyle name="Normal 25" xfId="443"/>
+    <cellStyle name="Normal 25 2" xfId="444"/>
+    <cellStyle name="Normal 26" xfId="445"/>
+    <cellStyle name="Normal 26 2" xfId="446"/>
+    <cellStyle name="Normal 27" xfId="447"/>
+    <cellStyle name="Normal 27 2" xfId="448"/>
+    <cellStyle name="Normal 28" xfId="449"/>
+    <cellStyle name="Normal 28 2" xfId="450"/>
+    <cellStyle name="Normal 29" xfId="451"/>
+    <cellStyle name="Normal 29 2" xfId="452"/>
+    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3 2" xfId="453"/>
+    <cellStyle name="Normal 3 2 2" xfId="454"/>
+    <cellStyle name="Normal 3 2 3" xfId="455"/>
+    <cellStyle name="Normal 3 2 4" xfId="456"/>
+    <cellStyle name="Normal 3 2 5" xfId="457"/>
+    <cellStyle name="Normal 3 2 6" xfId="458"/>
+    <cellStyle name="Normal 3 3" xfId="459"/>
+    <cellStyle name="Normal 3 3 2" xfId="460"/>
+    <cellStyle name="Normal 3 3 3" xfId="461"/>
+    <cellStyle name="Normal 3 4" xfId="462"/>
+    <cellStyle name="Normal 3 5" xfId="463"/>
+    <cellStyle name="Normal 3 6" xfId="464"/>
+    <cellStyle name="Normal 3 6 2" xfId="465"/>
+    <cellStyle name="Normal 3 6 3" xfId="466"/>
+    <cellStyle name="Normal 3 7" xfId="467"/>
+    <cellStyle name="Normal 3 8" xfId="468"/>
+    <cellStyle name="Normal 30" xfId="469"/>
+    <cellStyle name="Normal 30 2" xfId="470"/>
+    <cellStyle name="Normal 31" xfId="471"/>
+    <cellStyle name="Normal 31 2" xfId="472"/>
+    <cellStyle name="Normal 32" xfId="473"/>
+    <cellStyle name="Normal 32 2" xfId="474"/>
+    <cellStyle name="Normal 33" xfId="475"/>
+    <cellStyle name="Normal 33 2" xfId="476"/>
+    <cellStyle name="Normal 34" xfId="477"/>
+    <cellStyle name="Normal 34 2" xfId="478"/>
+    <cellStyle name="Normal 35" xfId="479"/>
+    <cellStyle name="Normal 35 2" xfId="480"/>
+    <cellStyle name="Normal 36" xfId="481"/>
+    <cellStyle name="Normal 36 2" xfId="482"/>
+    <cellStyle name="Normal 37" xfId="483"/>
+    <cellStyle name="Normal 37 2" xfId="484"/>
+    <cellStyle name="Normal 37 2 2" xfId="485"/>
+    <cellStyle name="Normal 37 3" xfId="486"/>
+    <cellStyle name="Normal 37 4" xfId="487"/>
+    <cellStyle name="Normal 37 5" xfId="488"/>
+    <cellStyle name="Normal 38" xfId="489"/>
+    <cellStyle name="Normal 38 2" xfId="490"/>
+    <cellStyle name="Normal 39" xfId="491"/>
+    <cellStyle name="Normal 39 2" xfId="492"/>
+    <cellStyle name="Normal 39 2 2" xfId="493"/>
+    <cellStyle name="Normal 39 3" xfId="494"/>
+    <cellStyle name="Normal 4" xfId="495"/>
+    <cellStyle name="Normal 4 2" xfId="496"/>
+    <cellStyle name="Normal 4 3" xfId="497"/>
+    <cellStyle name="Normal 4 3 2" xfId="498"/>
+    <cellStyle name="Normal 4 4" xfId="499"/>
+    <cellStyle name="Normal 40" xfId="500"/>
+    <cellStyle name="Normal 40 2" xfId="501"/>
+    <cellStyle name="Normal 41" xfId="502"/>
+    <cellStyle name="Normal 41 2" xfId="503"/>
+    <cellStyle name="Normal 42" xfId="504"/>
+    <cellStyle name="Normal 42 2" xfId="505"/>
+    <cellStyle name="Normal 43" xfId="506"/>
+    <cellStyle name="Normal 43 2" xfId="507"/>
+    <cellStyle name="Normal 44" xfId="508"/>
+    <cellStyle name="Normal 44 2" xfId="509"/>
+    <cellStyle name="Normal 45" xfId="510"/>
+    <cellStyle name="Normal 45 2" xfId="511"/>
+    <cellStyle name="Normal 46" xfId="512"/>
+    <cellStyle name="Normal 46 2" xfId="513"/>
+    <cellStyle name="Normal 47" xfId="514"/>
+    <cellStyle name="Normal 47 2" xfId="515"/>
+    <cellStyle name="Normal 48" xfId="516"/>
+    <cellStyle name="Normal 48 2" xfId="517"/>
+    <cellStyle name="Normal 49" xfId="518"/>
+    <cellStyle name="Normal 49 2" xfId="519"/>
+    <cellStyle name="Normal 5" xfId="520"/>
+    <cellStyle name="Normal 5 2" xfId="521"/>
+    <cellStyle name="Normal 5 3" xfId="522"/>
+    <cellStyle name="Normal 5 3 2" xfId="523"/>
+    <cellStyle name="Normal 5 4" xfId="524"/>
+    <cellStyle name="Normal 50" xfId="525"/>
+    <cellStyle name="Normal 50 2" xfId="526"/>
+    <cellStyle name="Normal 51" xfId="527"/>
+    <cellStyle name="Normal 51 2" xfId="528"/>
+    <cellStyle name="Normal 52" xfId="529"/>
+    <cellStyle name="Normal 52 2" xfId="530"/>
+    <cellStyle name="Normal 53" xfId="531"/>
+    <cellStyle name="Normal 53 2" xfId="532"/>
+    <cellStyle name="Normal 54" xfId="533"/>
+    <cellStyle name="Normal 54 2" xfId="534"/>
+    <cellStyle name="Normal 55" xfId="535"/>
+    <cellStyle name="Normal 56" xfId="536"/>
+    <cellStyle name="Normal 6" xfId="537"/>
+    <cellStyle name="Normal 6 10" xfId="538"/>
+    <cellStyle name="Normal 6 11" xfId="539"/>
+    <cellStyle name="Normal 6 12" xfId="540"/>
+    <cellStyle name="Normal 6 2" xfId="541"/>
+    <cellStyle name="Normal 6 2 2" xfId="542"/>
+    <cellStyle name="Normal 6 2 3" xfId="543"/>
+    <cellStyle name="Normal 6 3" xfId="544"/>
+    <cellStyle name="Normal 6 4" xfId="545"/>
+    <cellStyle name="Normal 6 4 2" xfId="546"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="547"/>
+    <cellStyle name="Normal 6 4 2 2 2" xfId="548"/>
+    <cellStyle name="Normal 6 4 2 2 2 2" xfId="549"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="550"/>
+    <cellStyle name="Normal 6 4 2 2 2 3" xfId="551"/>
+    <cellStyle name="Normal 6 4 2 2 2 4" xfId="552"/>
+    <cellStyle name="Normal 6 4 2 2 2 5" xfId="553"/>
+    <cellStyle name="Normal 6 4 2 2 3" xfId="554"/>
+    <cellStyle name="Normal 6 4 2 2 3 2" xfId="555"/>
+    <cellStyle name="Normal 6 4 2 2 4" xfId="556"/>
+    <cellStyle name="Normal 6 4 2 2 5" xfId="557"/>
+    <cellStyle name="Normal 6 4 2 2 6" xfId="558"/>
+    <cellStyle name="Normal 6 4 2 3" xfId="559"/>
+    <cellStyle name="Normal 6 4 2 3 2" xfId="560"/>
+    <cellStyle name="Normal 6 4 2 3 2 2" xfId="561"/>
+    <cellStyle name="Normal 6 4 2 3 3" xfId="562"/>
+    <cellStyle name="Normal 6 4 2 3 4" xfId="563"/>
+    <cellStyle name="Normal 6 4 2 3 5" xfId="564"/>
+    <cellStyle name="Normal 6 4 2 4" xfId="565"/>
+    <cellStyle name="Normal 6 4 2 4 2" xfId="566"/>
+    <cellStyle name="Normal 6 4 2 5" xfId="567"/>
+    <cellStyle name="Normal 6 4 2 6" xfId="568"/>
+    <cellStyle name="Normal 6 4 2 7" xfId="569"/>
+    <cellStyle name="Normal 6 4 3" xfId="570"/>
+    <cellStyle name="Normal 6 4 3 2" xfId="571"/>
+    <cellStyle name="Normal 6 4 3 2 2" xfId="572"/>
+    <cellStyle name="Normal 6 4 3 2 2 2" xfId="573"/>
+    <cellStyle name="Normal 6 4 3 2 3" xfId="574"/>
+    <cellStyle name="Normal 6 4 3 2 4" xfId="575"/>
+    <cellStyle name="Normal 6 4 3 2 5" xfId="576"/>
+    <cellStyle name="Normal 6 4 3 3" xfId="577"/>
+    <cellStyle name="Normal 6 4 3 3 2" xfId="578"/>
+    <cellStyle name="Normal 6 4 3 4" xfId="579"/>
+    <cellStyle name="Normal 6 4 3 5" xfId="580"/>
+    <cellStyle name="Normal 6 4 3 6" xfId="581"/>
+    <cellStyle name="Normal 6 4 4" xfId="582"/>
+    <cellStyle name="Normal 6 4 4 2" xfId="583"/>
+    <cellStyle name="Normal 6 4 4 2 2" xfId="584"/>
+    <cellStyle name="Normal 6 4 4 3" xfId="585"/>
+    <cellStyle name="Normal 6 4 4 4" xfId="586"/>
+    <cellStyle name="Normal 6 4 4 5" xfId="587"/>
+    <cellStyle name="Normal 6 4 5" xfId="588"/>
+    <cellStyle name="Normal 6 4 5 2" xfId="589"/>
+    <cellStyle name="Normal 6 4 6" xfId="590"/>
+    <cellStyle name="Normal 6 4 7" xfId="591"/>
+    <cellStyle name="Normal 6 4 8" xfId="592"/>
+    <cellStyle name="Normal 6 5" xfId="593"/>
+    <cellStyle name="Normal 6 5 2" xfId="594"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="595"/>
+    <cellStyle name="Normal 6 5 2 2 2" xfId="596"/>
+    <cellStyle name="Normal 6 5 2 2 2 2" xfId="597"/>
+    <cellStyle name="Normal 6 5 2 2 3" xfId="598"/>
+    <cellStyle name="Normal 6 5 2 2 4" xfId="599"/>
+    <cellStyle name="Normal 6 5 2 2 5" xfId="600"/>
+    <cellStyle name="Normal 6 5 2 3" xfId="601"/>
+    <cellStyle name="Normal 6 5 2 3 2" xfId="602"/>
+    <cellStyle name="Normal 6 5 2 4" xfId="603"/>
+    <cellStyle name="Normal 6 5 2 5" xfId="604"/>
+    <cellStyle name="Normal 6 5 2 6" xfId="605"/>
+    <cellStyle name="Normal 6 5 3" xfId="606"/>
+    <cellStyle name="Normal 6 5 3 2" xfId="607"/>
+    <cellStyle name="Normal 6 5 3 2 2" xfId="608"/>
+    <cellStyle name="Normal 6 5 3 3" xfId="609"/>
+    <cellStyle name="Normal 6 5 3 4" xfId="610"/>
+    <cellStyle name="Normal 6 5 3 5" xfId="611"/>
+    <cellStyle name="Normal 6 5 4" xfId="612"/>
+    <cellStyle name="Normal 6 5 4 2" xfId="613"/>
+    <cellStyle name="Normal 6 5 5" xfId="614"/>
+    <cellStyle name="Normal 6 5 6" xfId="615"/>
+    <cellStyle name="Normal 6 5 7" xfId="616"/>
+    <cellStyle name="Normal 6 6" xfId="617"/>
+    <cellStyle name="Normal 6 6 2" xfId="618"/>
+    <cellStyle name="Normal 6 6 2 2" xfId="619"/>
+    <cellStyle name="Normal 6 6 2 2 2" xfId="620"/>
+    <cellStyle name="Normal 6 6 2 3" xfId="621"/>
+    <cellStyle name="Normal 6 6 2 4" xfId="622"/>
+    <cellStyle name="Normal 6 6 2 5" xfId="623"/>
+    <cellStyle name="Normal 6 6 3" xfId="624"/>
+    <cellStyle name="Normal 6 6 3 2" xfId="625"/>
+    <cellStyle name="Normal 6 6 4" xfId="626"/>
+    <cellStyle name="Normal 6 6 5" xfId="627"/>
+    <cellStyle name="Normal 6 6 6" xfId="628"/>
+    <cellStyle name="Normal 6 7" xfId="629"/>
+    <cellStyle name="Normal 6 7 2" xfId="630"/>
+    <cellStyle name="Normal 6 7 2 2" xfId="631"/>
+    <cellStyle name="Normal 6 7 3" xfId="632"/>
+    <cellStyle name="Normal 6 7 4" xfId="633"/>
+    <cellStyle name="Normal 6 7 5" xfId="634"/>
+    <cellStyle name="Normal 6 8" xfId="635"/>
+    <cellStyle name="Normal 6 9" xfId="636"/>
+    <cellStyle name="Normal 6 9 2" xfId="637"/>
+    <cellStyle name="Normal 7" xfId="638"/>
+    <cellStyle name="Normal 7 10" xfId="639"/>
+    <cellStyle name="Normal 7 11" xfId="640"/>
+    <cellStyle name="Normal 7 2" xfId="641"/>
+    <cellStyle name="Normal 7 2 2" xfId="642"/>
+    <cellStyle name="Normal 7 3" xfId="643"/>
+    <cellStyle name="Normal 7 3 2" xfId="644"/>
+    <cellStyle name="Normal 7 4" xfId="645"/>
+    <cellStyle name="Normal 7 4 2" xfId="646"/>
+    <cellStyle name="Normal 7 4 2 2" xfId="647"/>
+    <cellStyle name="Normal 7 4 2 2 2" xfId="648"/>
+    <cellStyle name="Normal 7 4 2 2 2 2" xfId="649"/>
+    <cellStyle name="Normal 7 4 2 2 2 2 2" xfId="650"/>
+    <cellStyle name="Normal 7 4 2 2 2 3" xfId="651"/>
+    <cellStyle name="Normal 7 4 2 2 2 4" xfId="652"/>
+    <cellStyle name="Normal 7 4 2 2 2 5" xfId="653"/>
+    <cellStyle name="Normal 7 4 2 2 3" xfId="654"/>
+    <cellStyle name="Normal 7 4 2 2 3 2" xfId="655"/>
+    <cellStyle name="Normal 7 4 2 2 4" xfId="656"/>
+    <cellStyle name="Normal 7 4 2 2 5" xfId="657"/>
+    <cellStyle name="Normal 7 4 2 2 6" xfId="658"/>
+    <cellStyle name="Normal 7 4 2 3" xfId="659"/>
+    <cellStyle name="Normal 7 4 2 3 2" xfId="660"/>
+    <cellStyle name="Normal 7 4 2 3 2 2" xfId="661"/>
+    <cellStyle name="Normal 7 4 2 3 3" xfId="662"/>
+    <cellStyle name="Normal 7 4 2 3 4" xfId="663"/>
+    <cellStyle name="Normal 7 4 2 3 5" xfId="664"/>
+    <cellStyle name="Normal 7 4 2 4" xfId="665"/>
+    <cellStyle name="Normal 7 4 2 4 2" xfId="666"/>
+    <cellStyle name="Normal 7 4 2 5" xfId="667"/>
+    <cellStyle name="Normal 7 4 2 6" xfId="668"/>
+    <cellStyle name="Normal 7 4 2 7" xfId="669"/>
+    <cellStyle name="Normal 7 4 3" xfId="670"/>
+    <cellStyle name="Normal 7 4 3 2" xfId="671"/>
+    <cellStyle name="Normal 7 4 3 2 2" xfId="672"/>
+    <cellStyle name="Normal 7 4 3 2 2 2" xfId="673"/>
+    <cellStyle name="Normal 7 4 3 2 3" xfId="674"/>
+    <cellStyle name="Normal 7 4 3 2 4" xfId="675"/>
+    <cellStyle name="Normal 7 4 3 2 5" xfId="676"/>
+    <cellStyle name="Normal 7 4 3 3" xfId="677"/>
+    <cellStyle name="Normal 7 4 3 3 2" xfId="678"/>
+    <cellStyle name="Normal 7 4 3 4" xfId="679"/>
+    <cellStyle name="Normal 7 4 3 5" xfId="680"/>
+    <cellStyle name="Normal 7 4 3 6" xfId="681"/>
+    <cellStyle name="Normal 7 4 4" xfId="682"/>
+    <cellStyle name="Normal 7 4 4 2" xfId="683"/>
+    <cellStyle name="Normal 7 4 4 2 2" xfId="684"/>
+    <cellStyle name="Normal 7 4 4 3" xfId="685"/>
+    <cellStyle name="Normal 7 4 4 4" xfId="686"/>
+    <cellStyle name="Normal 7 4 4 5" xfId="687"/>
+    <cellStyle name="Normal 7 4 5" xfId="688"/>
+    <cellStyle name="Normal 7 4 5 2" xfId="689"/>
+    <cellStyle name="Normal 7 4 6" xfId="690"/>
+    <cellStyle name="Normal 7 4 7" xfId="691"/>
+    <cellStyle name="Normal 7 4 8" xfId="692"/>
+    <cellStyle name="Normal 7 5" xfId="693"/>
+    <cellStyle name="Normal 7 5 2" xfId="694"/>
+    <cellStyle name="Normal 7 5 2 2" xfId="695"/>
+    <cellStyle name="Normal 7 5 2 2 2" xfId="696"/>
+    <cellStyle name="Normal 7 5 2 2 2 2" xfId="697"/>
+    <cellStyle name="Normal 7 5 2 2 3" xfId="698"/>
+    <cellStyle name="Normal 7 5 2 2 4" xfId="699"/>
+    <cellStyle name="Normal 7 5 2 2 5" xfId="700"/>
+    <cellStyle name="Normal 7 5 2 3" xfId="701"/>
+    <cellStyle name="Normal 7 5 2 3 2" xfId="702"/>
+    <cellStyle name="Normal 7 5 2 4" xfId="703"/>
+    <cellStyle name="Normal 7 5 2 5" xfId="704"/>
+    <cellStyle name="Normal 7 5 2 6" xfId="705"/>
+    <cellStyle name="Normal 7 5 3" xfId="706"/>
+    <cellStyle name="Normal 7 5 3 2" xfId="707"/>
+    <cellStyle name="Normal 7 5 3 2 2" xfId="708"/>
+    <cellStyle name="Normal 7 5 3 3" xfId="709"/>
+    <cellStyle name="Normal 7 5 3 4" xfId="710"/>
+    <cellStyle name="Normal 7 5 3 5" xfId="711"/>
+    <cellStyle name="Normal 7 5 4" xfId="712"/>
+    <cellStyle name="Normal 7 5 4 2" xfId="713"/>
+    <cellStyle name="Normal 7 5 5" xfId="714"/>
+    <cellStyle name="Normal 7 5 6" xfId="715"/>
+    <cellStyle name="Normal 7 5 7" xfId="716"/>
+    <cellStyle name="Normal 7 6" xfId="717"/>
+    <cellStyle name="Normal 7 6 2" xfId="718"/>
+    <cellStyle name="Normal 7 6 2 2" xfId="719"/>
+    <cellStyle name="Normal 7 6 2 2 2" xfId="720"/>
+    <cellStyle name="Normal 7 6 2 3" xfId="721"/>
+    <cellStyle name="Normal 7 6 2 4" xfId="722"/>
+    <cellStyle name="Normal 7 6 2 5" xfId="723"/>
+    <cellStyle name="Normal 7 6 3" xfId="724"/>
+    <cellStyle name="Normal 7 6 3 2" xfId="725"/>
+    <cellStyle name="Normal 7 6 4" xfId="726"/>
+    <cellStyle name="Normal 7 6 5" xfId="727"/>
+    <cellStyle name="Normal 7 6 6" xfId="728"/>
+    <cellStyle name="Normal 7 7" xfId="729"/>
+    <cellStyle name="Normal 7 7 2" xfId="730"/>
+    <cellStyle name="Normal 7 7 2 2" xfId="731"/>
+    <cellStyle name="Normal 7 7 3" xfId="732"/>
+    <cellStyle name="Normal 7 7 4" xfId="733"/>
+    <cellStyle name="Normal 7 7 5" xfId="734"/>
+    <cellStyle name="Normal 7 8" xfId="735"/>
+    <cellStyle name="Normal 7 8 2" xfId="736"/>
+    <cellStyle name="Normal 7 9" xfId="737"/>
+    <cellStyle name="Normal 8" xfId="738"/>
+    <cellStyle name="Normal 8 2" xfId="739"/>
+    <cellStyle name="Normal 9" xfId="740"/>
+    <cellStyle name="Normal 9 2" xfId="741"/>
     <cellStyle name="Note" xfId="882" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note 2" xfId="742" xr:uid="{00000000-0005-0000-0000-00000D030000}"/>
-    <cellStyle name="Note 2 2" xfId="743" xr:uid="{00000000-0005-0000-0000-00000E030000}"/>
-    <cellStyle name="Note 2 2 2" xfId="911" xr:uid="{00000000-0005-0000-0000-00000F030000}"/>
+    <cellStyle name="Note 2" xfId="742"/>
+    <cellStyle name="Note 2 2" xfId="743"/>
+    <cellStyle name="Note 2 2 2" xfId="911"/>
     <cellStyle name="Output" xfId="877" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Output 2" xfId="744" xr:uid="{00000000-0005-0000-0000-000011030000}"/>
-    <cellStyle name="Output 2 2" xfId="745" xr:uid="{00000000-0005-0000-0000-000012030000}"/>
-    <cellStyle name="Output 2 2 2" xfId="912" xr:uid="{00000000-0005-0000-0000-000013030000}"/>
-    <cellStyle name="Percent 2" xfId="746" xr:uid="{00000000-0005-0000-0000-000014030000}"/>
-    <cellStyle name="Percent 2 2" xfId="747" xr:uid="{00000000-0005-0000-0000-000015030000}"/>
-    <cellStyle name="Percent 2 2 2" xfId="748" xr:uid="{00000000-0005-0000-0000-000016030000}"/>
-    <cellStyle name="Percent 2 2 3" xfId="749" xr:uid="{00000000-0005-0000-0000-000017030000}"/>
-    <cellStyle name="Percent 2 3" xfId="750" xr:uid="{00000000-0005-0000-0000-000018030000}"/>
-    <cellStyle name="Percent 2 4" xfId="751" xr:uid="{00000000-0005-0000-0000-000019030000}"/>
-    <cellStyle name="Percent 2 4 2" xfId="752" xr:uid="{00000000-0005-0000-0000-00001A030000}"/>
-    <cellStyle name="Percent 2 4 3" xfId="753" xr:uid="{00000000-0005-0000-0000-00001B030000}"/>
-    <cellStyle name="Percent 2 5" xfId="754" xr:uid="{00000000-0005-0000-0000-00001C030000}"/>
-    <cellStyle name="Percent 3" xfId="755" xr:uid="{00000000-0005-0000-0000-00001D030000}"/>
-    <cellStyle name="Percent 3 10" xfId="756" xr:uid="{00000000-0005-0000-0000-00001E030000}"/>
-    <cellStyle name="Percent 3 2" xfId="757" xr:uid="{00000000-0005-0000-0000-00001F030000}"/>
-    <cellStyle name="Percent 3 2 2" xfId="758" xr:uid="{00000000-0005-0000-0000-000020030000}"/>
-    <cellStyle name="Percent 3 2 2 2" xfId="759" xr:uid="{00000000-0005-0000-0000-000021030000}"/>
-    <cellStyle name="Percent 3 2 2 2 2" xfId="760" xr:uid="{00000000-0005-0000-0000-000022030000}"/>
-    <cellStyle name="Percent 3 2 2 2 2 2" xfId="761" xr:uid="{00000000-0005-0000-0000-000023030000}"/>
-    <cellStyle name="Percent 3 2 2 2 2 2 2" xfId="762" xr:uid="{00000000-0005-0000-0000-000024030000}"/>
-    <cellStyle name="Percent 3 2 2 2 2 3" xfId="763" xr:uid="{00000000-0005-0000-0000-000025030000}"/>
-    <cellStyle name="Percent 3 2 2 2 2 4" xfId="764" xr:uid="{00000000-0005-0000-0000-000026030000}"/>
-    <cellStyle name="Percent 3 2 2 2 2 5" xfId="765" xr:uid="{00000000-0005-0000-0000-000027030000}"/>
-    <cellStyle name="Percent 3 2 2 2 3" xfId="766" xr:uid="{00000000-0005-0000-0000-000028030000}"/>
-    <cellStyle name="Percent 3 2 2 2 3 2" xfId="767" xr:uid="{00000000-0005-0000-0000-000029030000}"/>
-    <cellStyle name="Percent 3 2 2 2 4" xfId="768" xr:uid="{00000000-0005-0000-0000-00002A030000}"/>
-    <cellStyle name="Percent 3 2 2 2 5" xfId="769" xr:uid="{00000000-0005-0000-0000-00002B030000}"/>
-    <cellStyle name="Percent 3 2 2 2 6" xfId="770" xr:uid="{00000000-0005-0000-0000-00002C030000}"/>
-    <cellStyle name="Percent 3 2 2 3" xfId="771" xr:uid="{00000000-0005-0000-0000-00002D030000}"/>
-    <cellStyle name="Percent 3 2 2 3 2" xfId="772" xr:uid="{00000000-0005-0000-0000-00002E030000}"/>
-    <cellStyle name="Percent 3 2 2 3 2 2" xfId="773" xr:uid="{00000000-0005-0000-0000-00002F030000}"/>
-    <cellStyle name="Percent 3 2 2 3 3" xfId="774" xr:uid="{00000000-0005-0000-0000-000030030000}"/>
-    <cellStyle name="Percent 3 2 2 3 4" xfId="775" xr:uid="{00000000-0005-0000-0000-000031030000}"/>
-    <cellStyle name="Percent 3 2 2 3 5" xfId="776" xr:uid="{00000000-0005-0000-0000-000032030000}"/>
-    <cellStyle name="Percent 3 2 2 4" xfId="777" xr:uid="{00000000-0005-0000-0000-000033030000}"/>
-    <cellStyle name="Percent 3 2 2 4 2" xfId="778" xr:uid="{00000000-0005-0000-0000-000034030000}"/>
-    <cellStyle name="Percent 3 2 2 5" xfId="779" xr:uid="{00000000-0005-0000-0000-000035030000}"/>
-    <cellStyle name="Percent 3 2 2 6" xfId="780" xr:uid="{00000000-0005-0000-0000-000036030000}"/>
-    <cellStyle name="Percent 3 2 2 7" xfId="781" xr:uid="{00000000-0005-0000-0000-000037030000}"/>
-    <cellStyle name="Percent 3 2 3" xfId="782" xr:uid="{00000000-0005-0000-0000-000038030000}"/>
-    <cellStyle name="Percent 3 2 3 2" xfId="783" xr:uid="{00000000-0005-0000-0000-000039030000}"/>
-    <cellStyle name="Percent 3 2 3 2 2" xfId="784" xr:uid="{00000000-0005-0000-0000-00003A030000}"/>
-    <cellStyle name="Percent 3 2 3 2 2 2" xfId="785" xr:uid="{00000000-0005-0000-0000-00003B030000}"/>
-    <cellStyle name="Percent 3 2 3 2 3" xfId="786" xr:uid="{00000000-0005-0000-0000-00003C030000}"/>
-    <cellStyle name="Percent 3 2 3 2 4" xfId="787" xr:uid="{00000000-0005-0000-0000-00003D030000}"/>
-    <cellStyle name="Percent 3 2 3 2 5" xfId="788" xr:uid="{00000000-0005-0000-0000-00003E030000}"/>
-    <cellStyle name="Percent 3 2 3 3" xfId="789" xr:uid="{00000000-0005-0000-0000-00003F030000}"/>
-    <cellStyle name="Percent 3 2 3 3 2" xfId="790" xr:uid="{00000000-0005-0000-0000-000040030000}"/>
-    <cellStyle name="Percent 3 2 3 4" xfId="791" xr:uid="{00000000-0005-0000-0000-000041030000}"/>
-    <cellStyle name="Percent 3 2 3 5" xfId="792" xr:uid="{00000000-0005-0000-0000-000042030000}"/>
-    <cellStyle name="Percent 3 2 3 6" xfId="793" xr:uid="{00000000-0005-0000-0000-000043030000}"/>
-    <cellStyle name="Percent 3 2 4" xfId="794" xr:uid="{00000000-0005-0000-0000-000044030000}"/>
-    <cellStyle name="Percent 3 2 4 2" xfId="795" xr:uid="{00000000-0005-0000-0000-000045030000}"/>
-    <cellStyle name="Percent 3 2 4 2 2" xfId="796" xr:uid="{00000000-0005-0000-0000-000046030000}"/>
-    <cellStyle name="Percent 3 2 4 3" xfId="797" xr:uid="{00000000-0005-0000-0000-000047030000}"/>
-    <cellStyle name="Percent 3 2 4 4" xfId="798" xr:uid="{00000000-0005-0000-0000-000048030000}"/>
-    <cellStyle name="Percent 3 2 4 5" xfId="799" xr:uid="{00000000-0005-0000-0000-000049030000}"/>
-    <cellStyle name="Percent 3 2 5" xfId="800" xr:uid="{00000000-0005-0000-0000-00004A030000}"/>
-    <cellStyle name="Percent 3 2 5 2" xfId="801" xr:uid="{00000000-0005-0000-0000-00004B030000}"/>
-    <cellStyle name="Percent 3 2 6" xfId="802" xr:uid="{00000000-0005-0000-0000-00004C030000}"/>
-    <cellStyle name="Percent 3 2 7" xfId="803" xr:uid="{00000000-0005-0000-0000-00004D030000}"/>
-    <cellStyle name="Percent 3 2 8" xfId="804" xr:uid="{00000000-0005-0000-0000-00004E030000}"/>
-    <cellStyle name="Percent 3 3" xfId="805" xr:uid="{00000000-0005-0000-0000-00004F030000}"/>
-    <cellStyle name="Percent 3 3 2" xfId="806" xr:uid="{00000000-0005-0000-0000-000050030000}"/>
-    <cellStyle name="Percent 3 3 2 2" xfId="807" xr:uid="{00000000-0005-0000-0000-000051030000}"/>
-    <cellStyle name="Percent 3 3 2 2 2" xfId="808" xr:uid="{00000000-0005-0000-0000-000052030000}"/>
-    <cellStyle name="Percent 3 3 2 2 2 2" xfId="809" xr:uid="{00000000-0005-0000-0000-000053030000}"/>
-    <cellStyle name="Percent 3 3 2 2 3" xfId="810" xr:uid="{00000000-0005-0000-0000-000054030000}"/>
-    <cellStyle name="Percent 3 3 2 2 4" xfId="811" xr:uid="{00000000-0005-0000-0000-000055030000}"/>
-    <cellStyle name="Percent 3 3 2 2 5" xfId="812" xr:uid="{00000000-0005-0000-0000-000056030000}"/>
-    <cellStyle name="Percent 3 3 2 3" xfId="813" xr:uid="{00000000-0005-0000-0000-000057030000}"/>
-    <cellStyle name="Percent 3 3 2 3 2" xfId="814" xr:uid="{00000000-0005-0000-0000-000058030000}"/>
-    <cellStyle name="Percent 3 3 2 4" xfId="815" xr:uid="{00000000-0005-0000-0000-000059030000}"/>
-    <cellStyle name="Percent 3 3 2 5" xfId="816" xr:uid="{00000000-0005-0000-0000-00005A030000}"/>
-    <cellStyle name="Percent 3 3 2 6" xfId="817" xr:uid="{00000000-0005-0000-0000-00005B030000}"/>
-    <cellStyle name="Percent 3 3 3" xfId="818" xr:uid="{00000000-0005-0000-0000-00005C030000}"/>
-    <cellStyle name="Percent 3 3 3 2" xfId="819" xr:uid="{00000000-0005-0000-0000-00005D030000}"/>
-    <cellStyle name="Percent 3 3 3 2 2" xfId="820" xr:uid="{00000000-0005-0000-0000-00005E030000}"/>
-    <cellStyle name="Percent 3 3 3 3" xfId="821" xr:uid="{00000000-0005-0000-0000-00005F030000}"/>
-    <cellStyle name="Percent 3 3 3 4" xfId="822" xr:uid="{00000000-0005-0000-0000-000060030000}"/>
-    <cellStyle name="Percent 3 3 3 5" xfId="823" xr:uid="{00000000-0005-0000-0000-000061030000}"/>
-    <cellStyle name="Percent 3 3 4" xfId="824" xr:uid="{00000000-0005-0000-0000-000062030000}"/>
-    <cellStyle name="Percent 3 3 4 2" xfId="825" xr:uid="{00000000-0005-0000-0000-000063030000}"/>
-    <cellStyle name="Percent 3 3 5" xfId="826" xr:uid="{00000000-0005-0000-0000-000064030000}"/>
-    <cellStyle name="Percent 3 3 6" xfId="827" xr:uid="{00000000-0005-0000-0000-000065030000}"/>
-    <cellStyle name="Percent 3 3 7" xfId="828" xr:uid="{00000000-0005-0000-0000-000066030000}"/>
-    <cellStyle name="Percent 3 4" xfId="829" xr:uid="{00000000-0005-0000-0000-000067030000}"/>
-    <cellStyle name="Percent 3 4 2" xfId="830" xr:uid="{00000000-0005-0000-0000-000068030000}"/>
-    <cellStyle name="Percent 3 4 2 2" xfId="831" xr:uid="{00000000-0005-0000-0000-000069030000}"/>
-    <cellStyle name="Percent 3 4 2 2 2" xfId="832" xr:uid="{00000000-0005-0000-0000-00006A030000}"/>
-    <cellStyle name="Percent 3 4 2 3" xfId="833" xr:uid="{00000000-0005-0000-0000-00006B030000}"/>
-    <cellStyle name="Percent 3 4 2 4" xfId="834" xr:uid="{00000000-0005-0000-0000-00006C030000}"/>
-    <cellStyle name="Percent 3 4 2 5" xfId="835" xr:uid="{00000000-0005-0000-0000-00006D030000}"/>
-    <cellStyle name="Percent 3 4 3" xfId="836" xr:uid="{00000000-0005-0000-0000-00006E030000}"/>
-    <cellStyle name="Percent 3 4 3 2" xfId="837" xr:uid="{00000000-0005-0000-0000-00006F030000}"/>
-    <cellStyle name="Percent 3 4 4" xfId="838" xr:uid="{00000000-0005-0000-0000-000070030000}"/>
-    <cellStyle name="Percent 3 4 5" xfId="839" xr:uid="{00000000-0005-0000-0000-000071030000}"/>
-    <cellStyle name="Percent 3 4 6" xfId="840" xr:uid="{00000000-0005-0000-0000-000072030000}"/>
-    <cellStyle name="Percent 3 5" xfId="841" xr:uid="{00000000-0005-0000-0000-000073030000}"/>
-    <cellStyle name="Percent 3 5 2" xfId="842" xr:uid="{00000000-0005-0000-0000-000074030000}"/>
-    <cellStyle name="Percent 3 5 2 2" xfId="843" xr:uid="{00000000-0005-0000-0000-000075030000}"/>
-    <cellStyle name="Percent 3 5 3" xfId="844" xr:uid="{00000000-0005-0000-0000-000076030000}"/>
-    <cellStyle name="Percent 3 5 4" xfId="845" xr:uid="{00000000-0005-0000-0000-000077030000}"/>
-    <cellStyle name="Percent 3 5 5" xfId="846" xr:uid="{00000000-0005-0000-0000-000078030000}"/>
-    <cellStyle name="Percent 3 6" xfId="847" xr:uid="{00000000-0005-0000-0000-000079030000}"/>
-    <cellStyle name="Percent 3 7" xfId="848" xr:uid="{00000000-0005-0000-0000-00007A030000}"/>
-    <cellStyle name="Percent 3 7 2" xfId="849" xr:uid="{00000000-0005-0000-0000-00007B030000}"/>
-    <cellStyle name="Percent 3 8" xfId="850" xr:uid="{00000000-0005-0000-0000-00007C030000}"/>
-    <cellStyle name="Percent 3 9" xfId="851" xr:uid="{00000000-0005-0000-0000-00007D030000}"/>
-    <cellStyle name="Percent 4" xfId="852" xr:uid="{00000000-0005-0000-0000-00007E030000}"/>
-    <cellStyle name="Percent 5" xfId="853" xr:uid="{00000000-0005-0000-0000-00007F030000}"/>
-    <cellStyle name="Percent 6" xfId="854" xr:uid="{00000000-0005-0000-0000-000080030000}"/>
-    <cellStyle name="PERCENT0" xfId="855" xr:uid="{00000000-0005-0000-0000-000081030000}"/>
-    <cellStyle name="PERCENT1" xfId="856" xr:uid="{00000000-0005-0000-0000-000082030000}"/>
-    <cellStyle name="PERCENT1 2" xfId="857" xr:uid="{00000000-0005-0000-0000-000083030000}"/>
-    <cellStyle name="PERCENT1 2 2" xfId="858" xr:uid="{00000000-0005-0000-0000-000084030000}"/>
-    <cellStyle name="PERCENT1 2 3" xfId="859" xr:uid="{00000000-0005-0000-0000-000085030000}"/>
+    <cellStyle name="Output 2" xfId="744"/>
+    <cellStyle name="Output 2 2" xfId="745"/>
+    <cellStyle name="Output 2 2 2" xfId="912"/>
+    <cellStyle name="Percent 2" xfId="746"/>
+    <cellStyle name="Percent 2 2" xfId="747"/>
+    <cellStyle name="Percent 2 2 2" xfId="748"/>
+    <cellStyle name="Percent 2 2 3" xfId="749"/>
+    <cellStyle name="Percent 2 3" xfId="750"/>
+    <cellStyle name="Percent 2 4" xfId="751"/>
+    <cellStyle name="Percent 2 4 2" xfId="752"/>
+    <cellStyle name="Percent 2 4 3" xfId="753"/>
+    <cellStyle name="Percent 2 5" xfId="754"/>
+    <cellStyle name="Percent 3" xfId="755"/>
+    <cellStyle name="Percent 3 10" xfId="756"/>
+    <cellStyle name="Percent 3 2" xfId="757"/>
+    <cellStyle name="Percent 3 2 2" xfId="758"/>
+    <cellStyle name="Percent 3 2 2 2" xfId="759"/>
+    <cellStyle name="Percent 3 2 2 2 2" xfId="760"/>
+    <cellStyle name="Percent 3 2 2 2 2 2" xfId="761"/>
+    <cellStyle name="Percent 3 2 2 2 2 2 2" xfId="762"/>
+    <cellStyle name="Percent 3 2 2 2 2 3" xfId="763"/>
+    <cellStyle name="Percent 3 2 2 2 2 4" xfId="764"/>
+    <cellStyle name="Percent 3 2 2 2 2 5" xfId="765"/>
+    <cellStyle name="Percent 3 2 2 2 3" xfId="766"/>
+    <cellStyle name="Percent 3 2 2 2 3 2" xfId="767"/>
+    <cellStyle name="Percent 3 2 2 2 4" xfId="768"/>
+    <cellStyle name="Percent 3 2 2 2 5" xfId="769"/>
+    <cellStyle name="Percent 3 2 2 2 6" xfId="770"/>
+    <cellStyle name="Percent 3 2 2 3" xfId="771"/>
+    <cellStyle name="Percent 3 2 2 3 2" xfId="772"/>
+    <cellStyle name="Percent 3 2 2 3 2 2" xfId="773"/>
+    <cellStyle name="Percent 3 2 2 3 3" xfId="774"/>
+    <cellStyle name="Percent 3 2 2 3 4" xfId="775"/>
+    <cellStyle name="Percent 3 2 2 3 5" xfId="776"/>
+    <cellStyle name="Percent 3 2 2 4" xfId="777"/>
+    <cellStyle name="Percent 3 2 2 4 2" xfId="778"/>
+    <cellStyle name="Percent 3 2 2 5" xfId="779"/>
+    <cellStyle name="Percent 3 2 2 6" xfId="780"/>
+    <cellStyle name="Percent 3 2 2 7" xfId="781"/>
+    <cellStyle name="Percent 3 2 3" xfId="782"/>
+    <cellStyle name="Percent 3 2 3 2" xfId="783"/>
+    <cellStyle name="Percent 3 2 3 2 2" xfId="784"/>
+    <cellStyle name="Percent 3 2 3 2 2 2" xfId="785"/>
+    <cellStyle name="Percent 3 2 3 2 3" xfId="786"/>
+    <cellStyle name="Percent 3 2 3 2 4" xfId="787"/>
+    <cellStyle name="Percent 3 2 3 2 5" xfId="788"/>
+    <cellStyle name="Percent 3 2 3 3" xfId="789"/>
+    <cellStyle name="Percent 3 2 3 3 2" xfId="790"/>
+    <cellStyle name="Percent 3 2 3 4" xfId="791"/>
+    <cellStyle name="Percent 3 2 3 5" xfId="792"/>
+    <cellStyle name="Percent 3 2 3 6" xfId="793"/>
+    <cellStyle name="Percent 3 2 4" xfId="794"/>
+    <cellStyle name="Percent 3 2 4 2" xfId="795"/>
+    <cellStyle name="Percent 3 2 4 2 2" xfId="796"/>
+    <cellStyle name="Percent 3 2 4 3" xfId="797"/>
+    <cellStyle name="Percent 3 2 4 4" xfId="798"/>
+    <cellStyle name="Percent 3 2 4 5" xfId="799"/>
+    <cellStyle name="Percent 3 2 5" xfId="800"/>
+    <cellStyle name="Percent 3 2 5 2" xfId="801"/>
+    <cellStyle name="Percent 3 2 6" xfId="802"/>
+    <cellStyle name="Percent 3 2 7" xfId="803"/>
+    <cellStyle name="Percent 3 2 8" xfId="804"/>
+    <cellStyle name="Percent 3 3" xfId="805"/>
+    <cellStyle name="Percent 3 3 2" xfId="806"/>
+    <cellStyle name="Percent 3 3 2 2" xfId="807"/>
+    <cellStyle name="Percent 3 3 2 2 2" xfId="808"/>
+    <cellStyle name="Percent 3 3 2 2 2 2" xfId="809"/>
+    <cellStyle name="Percent 3 3 2 2 3" xfId="810"/>
+    <cellStyle name="Percent 3 3 2 2 4" xfId="811"/>
+    <cellStyle name="Percent 3 3 2 2 5" xfId="812"/>
+    <cellStyle name="Percent 3 3 2 3" xfId="813"/>
+    <cellStyle name="Percent 3 3 2 3 2" xfId="814"/>
+    <cellStyle name="Percent 3 3 2 4" xfId="815"/>
+    <cellStyle name="Percent 3 3 2 5" xfId="816"/>
+    <cellStyle name="Percent 3 3 2 6" xfId="817"/>
+    <cellStyle name="Percent 3 3 3" xfId="818"/>
+    <cellStyle name="Percent 3 3 3 2" xfId="819"/>
+    <cellStyle name="Percent 3 3 3 2 2" xfId="820"/>
+    <cellStyle name="Percent 3 3 3 3" xfId="821"/>
+    <cellStyle name="Percent 3 3 3 4" xfId="822"/>
+    <cellStyle name="Percent 3 3 3 5" xfId="823"/>
+    <cellStyle name="Percent 3 3 4" xfId="824"/>
+    <cellStyle name="Percent 3 3 4 2" xfId="825"/>
+    <cellStyle name="Percent 3 3 5" xfId="826"/>
+    <cellStyle name="Percent 3 3 6" xfId="827"/>
+    <cellStyle name="Percent 3 3 7" xfId="828"/>
+    <cellStyle name="Percent 3 4" xfId="829"/>
+    <cellStyle name="Percent 3 4 2" xfId="830"/>
+    <cellStyle name="Percent 3 4 2 2" xfId="831"/>
+    <cellStyle name="Percent 3 4 2 2 2" xfId="832"/>
+    <cellStyle name="Percent 3 4 2 3" xfId="833"/>
+    <cellStyle name="Percent 3 4 2 4" xfId="834"/>
+    <cellStyle name="Percent 3 4 2 5" xfId="835"/>
+    <cellStyle name="Percent 3 4 3" xfId="836"/>
+    <cellStyle name="Percent 3 4 3 2" xfId="837"/>
+    <cellStyle name="Percent 3 4 4" xfId="838"/>
+    <cellStyle name="Percent 3 4 5" xfId="839"/>
+    <cellStyle name="Percent 3 4 6" xfId="840"/>
+    <cellStyle name="Percent 3 5" xfId="841"/>
+    <cellStyle name="Percent 3 5 2" xfId="842"/>
+    <cellStyle name="Percent 3 5 2 2" xfId="843"/>
+    <cellStyle name="Percent 3 5 3" xfId="844"/>
+    <cellStyle name="Percent 3 5 4" xfId="845"/>
+    <cellStyle name="Percent 3 5 5" xfId="846"/>
+    <cellStyle name="Percent 3 6" xfId="847"/>
+    <cellStyle name="Percent 3 7" xfId="848"/>
+    <cellStyle name="Percent 3 7 2" xfId="849"/>
+    <cellStyle name="Percent 3 8" xfId="850"/>
+    <cellStyle name="Percent 3 9" xfId="851"/>
+    <cellStyle name="Percent 4" xfId="852"/>
+    <cellStyle name="Percent 5" xfId="853"/>
+    <cellStyle name="Percent 6" xfId="854"/>
+    <cellStyle name="PERCENT0" xfId="855"/>
+    <cellStyle name="PERCENT1" xfId="856"/>
+    <cellStyle name="PERCENT1 2" xfId="857"/>
+    <cellStyle name="PERCENT1 2 2" xfId="858"/>
+    <cellStyle name="PERCENT1 2 3" xfId="859"/>
     <cellStyle name="Title" xfId="868" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="title 1" xfId="860" xr:uid="{00000000-0005-0000-0000-000087030000}"/>
-    <cellStyle name="title 2" xfId="861" xr:uid="{00000000-0005-0000-0000-000088030000}"/>
-    <cellStyle name="Title 2 2" xfId="862" xr:uid="{00000000-0005-0000-0000-000089030000}"/>
-    <cellStyle name="title 3" xfId="863" xr:uid="{00000000-0005-0000-0000-00008A030000}"/>
+    <cellStyle name="title 1" xfId="860"/>
+    <cellStyle name="title 2" xfId="861"/>
+    <cellStyle name="Title 2 2" xfId="862"/>
+    <cellStyle name="title 3" xfId="863"/>
     <cellStyle name="Total" xfId="884" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Total 2" xfId="864" xr:uid="{00000000-0005-0000-0000-00008C030000}"/>
-    <cellStyle name="Total 2 2" xfId="865" xr:uid="{00000000-0005-0000-0000-00008D030000}"/>
-    <cellStyle name="Total 2 2 2" xfId="913" xr:uid="{00000000-0005-0000-0000-00008E030000}"/>
+    <cellStyle name="Total 2" xfId="864"/>
+    <cellStyle name="Total 2 2" xfId="865"/>
+    <cellStyle name="Total 2 2 2" xfId="913"/>
     <cellStyle name="Warning Text" xfId="881" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Warning Text 2" xfId="866" xr:uid="{00000000-0005-0000-0000-000090030000}"/>
-    <cellStyle name="Warning Text 2 2" xfId="867" xr:uid="{00000000-0005-0000-0000-000091030000}"/>
+    <cellStyle name="Warning Text 2" xfId="866"/>
+    <cellStyle name="Warning Text 2 2" xfId="867"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8648,7 +8651,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8681,26 +8684,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8733,23 +8719,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8925,24 +8894,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:F94"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D39" sqref="D39:D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:6">
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3" spans="3:6">
       <c r="C3" s="1" t="s">
@@ -9060,10 +9029,10 @@
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="3:6">
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="39"/>
+      <c r="D18" s="42"/>
     </row>
     <row r="19" spans="3:6">
       <c r="C19" s="1" t="s">
@@ -9398,10 +9367,10 @@
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="3:4">
-      <c r="C60" s="38" t="s">
+      <c r="C60" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D60" s="39"/>
+      <c r="D60" s="42"/>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="1" t="s">
@@ -9544,10 +9513,10 @@
       <c r="D77" s="3"/>
     </row>
     <row r="78" spans="3:5">
-      <c r="C78" s="38" t="s">
+      <c r="C78" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D78" s="39"/>
+      <c r="D78" s="42"/>
     </row>
     <row r="79" spans="3:5">
       <c r="C79" s="1" t="s">
@@ -9606,10 +9575,10 @@
       <c r="D86" s="3"/>
     </row>
     <row r="87" spans="3:4">
-      <c r="C87" s="38" t="s">
+      <c r="C87" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="D87" s="39"/>
+      <c r="D87" s="42"/>
     </row>
     <row r="88" spans="3:4">
       <c r="C88" s="1" t="s">
@@ -9665,16 +9634,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E335"/>
   <sheetViews>
     <sheetView topLeftCell="A169" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="42.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
@@ -11170,35 +11139,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E175481E-5C55-2F4B-B0E6-A653B929C7D6}">
-  <dimension ref="B2:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="43" t="s">
         <v>392</v>
       </c>
-      <c r="C2" s="40"/>
+      <c r="C2" s="43"/>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="36" t="s">
         <v>393</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="37" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="38" t="s">
         <v>395</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="37" t="s">
         <v>396</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="C5" s="26"/>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>